<commit_message>
severos cambios tan tuntunsahur
</commit_message>
<xml_diff>
--- a/templates/plantilla.xlsx
+++ b/templates/plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pract06.desarrollo\OneDrive - Coopidrogas\Escritorio\camunda_back\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{C903F4BE-FECE-4BB5-A2A7-51C7DBF94218}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6A2AD5F-FF31-4DD4-9581-654843C71EF8}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{C903F4BE-FECE-4BB5-A2A7-51C7DBF94218}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5C8A0AD-0841-42A6-98E7-891AA03486BD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{6CC2AB2B-0F37-47AE-B363-6A70476DA6B2}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
   <si>
     <t xml:space="preserve">REQUISICIÓN DE COMPRA O SERVICIO  </t>
   </si>
@@ -257,24 +257,6 @@
     <t>FIRMA:</t>
   </si>
   <si>
-    <t>AUTORIZACIÓN GERENCIA GENERAL (en caso que aplique)</t>
-  </si>
-  <si>
-    <t>RECEPCIÓN COMPRAS INSTITUCIONALES</t>
-  </si>
-  <si>
-    <t>FECHA</t>
-  </si>
-  <si>
-    <t>HORA</t>
-  </si>
-  <si>
-    <t>CONSECUTIVO</t>
-  </si>
-  <si>
-    <t>FIRMA</t>
-  </si>
-  <si>
     <t>CONSIDERACIONES ESPECIALES:
 1.Si la compra del bien o servicio requiere validación por parte del área de SST, el área solicitante debe confirmar el concepto para los casos que aplique y solicitar aprobacion de la Jefatura de SST.
 2.Toda solicitud de hadware y software (equipos tecnológico, licencias de software, mouse, teclado, multipuertos, diadema, etc.), debe pasar por aprobación de la gerencia de tecnología y proyectos, previo a la formalización de la requisición al área de servicios administrativos.</t>
@@ -332,6 +314,15 @@
   </si>
   <si>
     <t>SI / NO</t>
+  </si>
+  <si>
+    <t>APROBACIÓN GERENCIA ADMINISTRATIVA (en caso que aplique)</t>
+  </si>
+  <si>
+    <t>APROBACIÓN GERENCIA GENERAL (en caso que aplique)</t>
+  </si>
+  <si>
+    <t>APROBACIÓNES</t>
   </si>
 </sst>
 </file>
@@ -411,7 +402,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -438,12 +429,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF002060"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -455,7 +440,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="62">
+  <borders count="64">
     <border>
       <left/>
       <right/>
@@ -895,36 +880,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -1200,11 +1159,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1257,38 +1260,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1393,242 +1402,80 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1696,16 +1543,16 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1714,59 +1561,183 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1785,14 +1756,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1860,13 +1823,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:colOff>224518</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>85692</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>368431</xdr:colOff>
+      <xdr:colOff>816429</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
@@ -1898,8 +1861,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="409575" y="285717"/>
-          <a:ext cx="2091742" cy="485808"/>
+          <a:off x="496661" y="317013"/>
+          <a:ext cx="2347232" cy="483087"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1912,278 +1875,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>78442</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>67236</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>313765</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>392206</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CuadroTexto 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8998324" y="2700618"/>
-          <a:ext cx="235323" cy="324970"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100">
-              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>SI</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>544607</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>73960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>33618</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>398930</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CuadroTexto 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9464489" y="2707342"/>
-          <a:ext cx="374276" cy="324970"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100">
-              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>NO</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>19</xdr:col>
-          <xdr:colOff>352425</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>20</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>438150</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2050" name="Check Box 2" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2050"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>20</xdr:col>
-          <xdr:colOff>238125</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>22</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>438150</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2051" name="Check Box 3" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2051"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003080000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -2525,78 +2216,78 @@
     </row>
     <row r="3" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="54" t="s">
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54" t="s">
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56"/>
       <c r="Q3" s="12"/>
     </row>
     <row r="4" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="11"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54" t="s">
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
-      <c r="O4" s="54"/>
-      <c r="P4" s="54"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="56"/>
       <c r="Q4" s="12"/>
     </row>
     <row r="5" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="11"/>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="55" t="s">
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="55"/>
-      <c r="O5" s="55"/>
-      <c r="P5" s="55"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="57"/>
+      <c r="P5" s="57"/>
       <c r="Q5" s="12"/>
     </row>
     <row r="6" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="51"/>
       <c r="K6" s="3" t="s">
         <v>5</v>
       </c>
@@ -2617,23 +2308,23 @@
     </row>
     <row r="8" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="11"/>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="I8" s="42" t="s">
+      <c r="D8" s="53"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="I8" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="42"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="43"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="43"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="45"/>
+      <c r="P8" s="45"/>
       <c r="Q8" s="12"/>
     </row>
     <row r="9" spans="2:17" ht="9" customHeight="1" x14ac:dyDescent="0.25">
@@ -2647,10 +2338,10 @@
     </row>
     <row r="10" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="11"/>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="51"/>
+      <c r="D10" s="53"/>
       <c r="E10" s="24"/>
       <c r="F10" s="15" t="s">
         <v>11</v>
@@ -2658,11 +2349,11 @@
       <c r="G10" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="42" t="s">
+      <c r="H10" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
       <c r="K10" s="16" t="s">
         <v>14</v>
       </c>
@@ -2680,31 +2371,31 @@
     </row>
     <row r="12" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="11"/>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="51"/>
+      <c r="D12" s="53"/>
       <c r="E12" s="24"/>
-      <c r="F12" s="42" t="s">
+      <c r="F12" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="42"/>
-      <c r="H12" s="43" t="s">
+      <c r="G12" s="44"/>
+      <c r="H12" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="43"/>
-      <c r="J12" s="42" t="s">
+      <c r="I12" s="45"/>
+      <c r="J12" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="43" t="str">
+      <c r="K12" s="44"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="45" t="str">
         <f>VLOOKUP(H12,Hoja3!B4:C7,2,FALSE)</f>
         <v>HASTA 5 DÍAS HÁBILES</v>
       </c>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="43"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="45"/>
+      <c r="P12" s="45"/>
       <c r="Q12" s="12"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
@@ -2713,58 +2404,58 @@
     </row>
     <row r="14" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11"/>
-      <c r="C14" s="73" t="s">
+      <c r="C14" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="73"/>
-      <c r="J14" s="73"/>
-      <c r="K14" s="73"/>
-      <c r="L14" s="73"/>
-      <c r="M14" s="73"/>
-      <c r="N14" s="73"/>
-      <c r="O14" s="73"/>
-      <c r="P14" s="73"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="75"/>
+      <c r="I14" s="75"/>
+      <c r="J14" s="75"/>
+      <c r="K14" s="75"/>
+      <c r="L14" s="75"/>
+      <c r="M14" s="75"/>
+      <c r="N14" s="75"/>
+      <c r="O14" s="75"/>
+      <c r="P14" s="75"/>
       <c r="Q14" s="12"/>
     </row>
     <row r="15" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="11"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="57"/>
-      <c r="M15" s="57"/>
-      <c r="N15" s="57"/>
-      <c r="O15" s="57"/>
-      <c r="P15" s="57"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="59"/>
+      <c r="N15" s="59"/>
+      <c r="O15" s="59"/>
+      <c r="P15" s="59"/>
       <c r="Q15" s="12"/>
     </row>
     <row r="16" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="11"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="57"/>
-      <c r="P16" s="57"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="59"/>
+      <c r="N16" s="59"/>
+      <c r="O16" s="59"/>
+      <c r="P16" s="59"/>
       <c r="Q16" s="12"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
@@ -2773,41 +2464,41 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="11"/>
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="50" t="s">
+      <c r="D18" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50" t="s">
+      <c r="E18" s="52"/>
+      <c r="F18" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="50" t="s">
+      <c r="G18" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="50" t="s">
+      <c r="H18" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="I18" s="50"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="50" t="s">
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="L18" s="50"/>
-      <c r="M18" s="50"/>
-      <c r="N18" s="50"/>
-      <c r="O18" s="50"/>
-      <c r="P18" s="50"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="52"/>
+      <c r="N18" s="52"/>
+      <c r="O18" s="52"/>
+      <c r="P18" s="52"/>
       <c r="Q18" s="12"/>
     </row>
     <row r="19" spans="2:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="11"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
       <c r="H19" s="1" t="s">
         <v>14</v>
       </c>
@@ -2817,210 +2508,210 @@
       <c r="J19" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K19" s="50"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="50"/>
-      <c r="O19" s="50"/>
-      <c r="P19" s="50"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="52"/>
+      <c r="O19" s="52"/>
+      <c r="P19" s="52"/>
       <c r="Q19" s="12"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="11"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="41"/>
-      <c r="P20" s="41"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
       <c r="Q20" s="12"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="11"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="41"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="41"/>
-      <c r="N21" s="41"/>
-      <c r="O21" s="41"/>
-      <c r="P21" s="41"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="43"/>
       <c r="Q21" s="12"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="41"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="43"/>
       <c r="Q22" s="12"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="41"/>
-      <c r="P23" s="41"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="43"/>
+      <c r="P23" s="43"/>
       <c r="Q23" s="12"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="11"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
-      <c r="P24" s="41"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="43"/>
+      <c r="P24" s="43"/>
       <c r="Q24" s="12"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="11"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="41"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="43"/>
+      <c r="P25" s="43"/>
       <c r="Q25" s="12"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="41"/>
-      <c r="P26" s="41"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
       <c r="Q26" s="12"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="11"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="41"/>
-      <c r="L27" s="41"/>
-      <c r="M27" s="41"/>
-      <c r="N27" s="41"/>
-      <c r="O27" s="41"/>
-      <c r="P27" s="41"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="43"/>
+      <c r="P27" s="43"/>
       <c r="Q27" s="12"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="11"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="41"/>
-      <c r="N28" s="41"/>
-      <c r="O28" s="41"/>
-      <c r="P28" s="41"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="43"/>
+      <c r="P28" s="43"/>
       <c r="Q28" s="12"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="11"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="41"/>
-      <c r="M29" s="41"/>
-      <c r="N29" s="41"/>
-      <c r="O29" s="41"/>
-      <c r="P29" s="41"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="43"/>
+      <c r="P29" s="43"/>
       <c r="Q29" s="12"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="11"/>
       <c r="C30" s="5"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="41"/>
-      <c r="M30" s="41"/>
-      <c r="N30" s="41"/>
-      <c r="O30" s="41"/>
-      <c r="P30" s="41"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="43"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="43"/>
+      <c r="P30" s="43"/>
       <c r="Q30" s="12"/>
     </row>
     <row r="31" spans="2:17" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3029,22 +2720,22 @@
     </row>
     <row r="32" spans="2:17" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="11"/>
-      <c r="C32" s="56" t="s">
+      <c r="C32" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="56"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="56"/>
-      <c r="K32" s="56"/>
-      <c r="L32" s="56"/>
-      <c r="M32" s="56"/>
-      <c r="N32" s="56"/>
-      <c r="O32" s="56"/>
-      <c r="P32" s="56"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="58"/>
+      <c r="J32" s="58"/>
+      <c r="K32" s="58"/>
+      <c r="L32" s="58"/>
+      <c r="M32" s="58"/>
+      <c r="N32" s="58"/>
+      <c r="O32" s="58"/>
+      <c r="P32" s="58"/>
       <c r="Q32" s="12"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
@@ -3053,76 +2744,76 @@
     </row>
     <row r="34" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="11"/>
-      <c r="C34" s="52" t="s">
+      <c r="C34" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="52"/>
-      <c r="L34" s="52"/>
-      <c r="M34" s="52"/>
-      <c r="N34" s="52"/>
-      <c r="O34" s="52"/>
-      <c r="P34" s="52"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="54"/>
+      <c r="H34" s="54"/>
+      <c r="I34" s="54"/>
+      <c r="J34" s="54"/>
+      <c r="K34" s="54"/>
+      <c r="L34" s="54"/>
+      <c r="M34" s="54"/>
+      <c r="N34" s="54"/>
+      <c r="O34" s="54"/>
+      <c r="P34" s="54"/>
       <c r="Q34" s="12"/>
     </row>
     <row r="35" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="11"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="40"/>
-      <c r="J35" s="40"/>
-      <c r="K35" s="40"/>
-      <c r="L35" s="40"/>
-      <c r="M35" s="40"/>
-      <c r="N35" s="40"/>
-      <c r="O35" s="40"/>
-      <c r="P35" s="40"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="42"/>
+      <c r="J35" s="42"/>
+      <c r="K35" s="42"/>
+      <c r="L35" s="42"/>
+      <c r="M35" s="42"/>
+      <c r="N35" s="42"/>
+      <c r="O35" s="42"/>
+      <c r="P35" s="42"/>
       <c r="Q35" s="12"/>
     </row>
     <row r="36" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="11"/>
-      <c r="C36" s="60"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="60"/>
-      <c r="F36" s="60"/>
-      <c r="G36" s="60"/>
-      <c r="H36" s="60"/>
-      <c r="I36" s="60"/>
-      <c r="J36" s="60"/>
-      <c r="K36" s="60"/>
-      <c r="L36" s="60"/>
-      <c r="M36" s="60"/>
-      <c r="N36" s="60"/>
-      <c r="O36" s="60"/>
-      <c r="P36" s="60"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="62"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="62"/>
+      <c r="J36" s="62"/>
+      <c r="K36" s="62"/>
+      <c r="L36" s="62"/>
+      <c r="M36" s="62"/>
+      <c r="N36" s="62"/>
+      <c r="O36" s="62"/>
+      <c r="P36" s="62"/>
       <c r="Q36" s="12"/>
     </row>
     <row r="37" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="11"/>
-      <c r="C37" s="60"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
-      <c r="G37" s="60"/>
-      <c r="H37" s="60"/>
-      <c r="I37" s="60"/>
-      <c r="J37" s="60"/>
-      <c r="K37" s="60"/>
-      <c r="L37" s="60"/>
-      <c r="M37" s="60"/>
-      <c r="N37" s="60"/>
-      <c r="O37" s="60"/>
-      <c r="P37" s="60"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="62"/>
+      <c r="I37" s="62"/>
+      <c r="J37" s="62"/>
+      <c r="K37" s="62"/>
+      <c r="L37" s="62"/>
+      <c r="M37" s="62"/>
+      <c r="N37" s="62"/>
+      <c r="O37" s="62"/>
+      <c r="P37" s="62"/>
       <c r="Q37" s="12"/>
       <c r="T37">
         <f>1546-1378</f>
@@ -3142,96 +2833,96 @@
     </row>
     <row r="40" spans="2:20" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="11"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="41"/>
-      <c r="H40" s="41"/>
-      <c r="I40" s="41"/>
-      <c r="J40" s="66"/>
-      <c r="K40" s="71"/>
-      <c r="L40" s="72"/>
-      <c r="M40" s="71"/>
-      <c r="N40" s="72"/>
-      <c r="O40" s="71"/>
-      <c r="P40" s="72"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="68"/>
+      <c r="K40" s="73"/>
+      <c r="L40" s="74"/>
+      <c r="M40" s="73"/>
+      <c r="N40" s="74"/>
+      <c r="O40" s="73"/>
+      <c r="P40" s="74"/>
       <c r="Q40" s="12"/>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B41" s="11"/>
-      <c r="C41" s="59" t="s">
+      <c r="C41" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="59"/>
-      <c r="E41" s="59" t="s">
+      <c r="D41" s="61"/>
+      <c r="E41" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="F41" s="59"/>
-      <c r="G41" s="59" t="s">
+      <c r="F41" s="61"/>
+      <c r="G41" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="H41" s="59"/>
-      <c r="I41" s="59"/>
-      <c r="J41" s="67"/>
-      <c r="K41" s="62" t="s">
+      <c r="H41" s="61"/>
+      <c r="I41" s="61"/>
+      <c r="J41" s="69"/>
+      <c r="K41" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="L41" s="63"/>
-      <c r="M41" s="62" t="s">
+      <c r="L41" s="65"/>
+      <c r="M41" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="N41" s="63"/>
-      <c r="O41" s="62" t="s">
+      <c r="N41" s="65"/>
+      <c r="O41" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="P41" s="63"/>
+      <c r="P41" s="65"/>
       <c r="Q41" s="12"/>
     </row>
     <row r="42" spans="2:20" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="11"/>
-      <c r="C42" s="59"/>
-      <c r="D42" s="59"/>
-      <c r="E42" s="59"/>
-      <c r="F42" s="59"/>
-      <c r="G42" s="59"/>
-      <c r="H42" s="59"/>
-      <c r="I42" s="59"/>
-      <c r="J42" s="64" t="s">
+      <c r="C42" s="61"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="61"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="61"/>
+      <c r="H42" s="61"/>
+      <c r="I42" s="61"/>
+      <c r="J42" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="K42" s="68"/>
-      <c r="L42" s="69"/>
-      <c r="M42" s="69"/>
-      <c r="N42" s="69"/>
-      <c r="O42" s="69"/>
-      <c r="P42" s="70"/>
+      <c r="K42" s="70"/>
+      <c r="L42" s="71"/>
+      <c r="M42" s="71"/>
+      <c r="N42" s="71"/>
+      <c r="O42" s="71"/>
+      <c r="P42" s="72"/>
       <c r="Q42" s="12"/>
     </row>
     <row r="43" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="11"/>
-      <c r="C43" s="59" t="s">
+      <c r="C43" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="D43" s="59"/>
-      <c r="E43" s="59" t="s">
+      <c r="D43" s="61"/>
+      <c r="E43" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F43" s="59"/>
-      <c r="G43" s="59" t="s">
+      <c r="F43" s="61"/>
+      <c r="G43" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="H43" s="59"/>
-      <c r="I43" s="59"/>
-      <c r="J43" s="65"/>
-      <c r="K43" s="68" t="s">
+      <c r="H43" s="61"/>
+      <c r="I43" s="61"/>
+      <c r="J43" s="67"/>
+      <c r="K43" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="L43" s="69"/>
-      <c r="M43" s="69"/>
-      <c r="N43" s="69"/>
-      <c r="O43" s="69"/>
-      <c r="P43" s="70"/>
+      <c r="L43" s="71"/>
+      <c r="M43" s="71"/>
+      <c r="N43" s="71"/>
+      <c r="O43" s="71"/>
+      <c r="P43" s="72"/>
       <c r="Q43" s="12"/>
     </row>
     <row r="44" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3245,11 +2936,11 @@
       <c r="I44" s="21"/>
       <c r="J44" s="22"/>
       <c r="K44" s="22"/>
-      <c r="L44" s="61"/>
-      <c r="M44" s="61"/>
-      <c r="N44" s="61"/>
-      <c r="O44" s="61"/>
-      <c r="P44" s="61"/>
+      <c r="L44" s="63"/>
+      <c r="M44" s="63"/>
+      <c r="N44" s="63"/>
+      <c r="O44" s="63"/>
+      <c r="P44" s="63"/>
       <c r="Q44" s="12"/>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
@@ -3258,22 +2949,22 @@
     </row>
     <row r="46" spans="2:20" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="11"/>
-      <c r="C46" s="58" t="s">
+      <c r="C46" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="D46" s="58"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="58"/>
-      <c r="H46" s="58"/>
-      <c r="I46" s="58"/>
-      <c r="J46" s="58"/>
-      <c r="K46" s="58"/>
-      <c r="L46" s="58"/>
-      <c r="M46" s="58"/>
-      <c r="N46" s="58"/>
-      <c r="O46" s="58"/>
-      <c r="P46" s="58"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="60"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="60"/>
+      <c r="H46" s="60"/>
+      <c r="I46" s="60"/>
+      <c r="J46" s="60"/>
+      <c r="K46" s="60"/>
+      <c r="L46" s="60"/>
+      <c r="M46" s="60"/>
+      <c r="N46" s="60"/>
+      <c r="O46" s="60"/>
+      <c r="P46" s="60"/>
       <c r="Q46" s="12"/>
     </row>
     <row r="47" spans="2:20" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3400,17 +3091,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF3B689-9F06-47C4-AF24-1D135A215254}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF3B689-9F06-47C4-AF24-1D135A215254}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W39"/>
+  <dimension ref="A1:W1167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18:P18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="17.25" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="148.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.140625" style="30" customWidth="1"/>
     <col min="2" max="2" width="10" style="28" customWidth="1"/>
@@ -3429,116 +3120,143 @@
     <col min="16" max="16" width="4" style="28" customWidth="1"/>
     <col min="17" max="17" width="18.85546875" style="28" customWidth="1"/>
     <col min="18" max="18" width="8.28515625" style="28" customWidth="1"/>
-    <col min="19" max="19" width="4.7109375" style="28" customWidth="1"/>
+    <col min="19" max="19" width="1.42578125" style="28" customWidth="1"/>
     <col min="20" max="20" width="9.5703125" style="28" customWidth="1"/>
     <col min="21" max="21" width="3.7109375" style="28" customWidth="1"/>
-    <col min="22" max="22" width="4.42578125" style="28" customWidth="1"/>
+    <col min="22" max="22" width="12" style="28" customWidth="1"/>
     <col min="23" max="23" width="4.7109375" style="30" customWidth="1"/>
     <col min="24" max="16384" width="11.42578125" style="28" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" s="30" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:23" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="171"/>
-      <c r="C2" s="172"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="153" t="s">
+    <row r="1" spans="1:22" s="184" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="30"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+    </row>
+    <row r="2" spans="1:22" s="184" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="30"/>
+      <c r="B2" s="119"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="154"/>
-      <c r="G2" s="154"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="154"/>
-      <c r="J2" s="154"/>
-      <c r="K2" s="154"/>
-      <c r="L2" s="155"/>
-      <c r="M2" s="165" t="s">
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="166"/>
-      <c r="O2" s="166"/>
-      <c r="P2" s="166"/>
-      <c r="Q2" s="166"/>
-      <c r="R2" s="166"/>
-      <c r="S2" s="166"/>
-      <c r="T2" s="166"/>
-      <c r="U2" s="166"/>
-      <c r="V2" s="167"/>
-    </row>
-    <row r="3" spans="2:23" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="174"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="156"/>
-      <c r="F3" s="157"/>
-      <c r="G3" s="157"/>
-      <c r="H3" s="157"/>
-      <c r="I3" s="157"/>
-      <c r="J3" s="157"/>
-      <c r="K3" s="157"/>
-      <c r="L3" s="158"/>
-      <c r="M3" s="165" t="s">
+      <c r="N2" s="114"/>
+      <c r="O2" s="114"/>
+      <c r="P2" s="114"/>
+      <c r="Q2" s="114"/>
+      <c r="R2" s="114"/>
+      <c r="S2" s="114"/>
+      <c r="T2" s="114"/>
+      <c r="U2" s="114"/>
+      <c r="V2" s="115"/>
+    </row>
+    <row r="3" spans="1:22" s="184" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="30"/>
+      <c r="B3" s="122"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="106"/>
+      <c r="M3" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="166"/>
-      <c r="O3" s="166"/>
-      <c r="P3" s="166"/>
-      <c r="Q3" s="166"/>
-      <c r="R3" s="166"/>
-      <c r="S3" s="166"/>
-      <c r="T3" s="166"/>
-      <c r="U3" s="166"/>
-      <c r="V3" s="167"/>
-    </row>
-    <row r="4" spans="2:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="159" t="s">
+      <c r="N3" s="114"/>
+      <c r="O3" s="114"/>
+      <c r="P3" s="114"/>
+      <c r="Q3" s="114"/>
+      <c r="R3" s="114"/>
+      <c r="S3" s="114"/>
+      <c r="T3" s="114"/>
+      <c r="U3" s="114"/>
+      <c r="V3" s="115"/>
+    </row>
+    <row r="4" spans="1:22" s="184" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="30"/>
+      <c r="B4" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="160"/>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
-      <c r="F4" s="160"/>
-      <c r="G4" s="160"/>
-      <c r="H4" s="160"/>
-      <c r="I4" s="160"/>
-      <c r="J4" s="160"/>
-      <c r="K4" s="160"/>
-      <c r="L4" s="161"/>
-      <c r="M4" s="168" t="s">
+      <c r="C4" s="108"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="108"/>
+      <c r="G4" s="108"/>
+      <c r="H4" s="108"/>
+      <c r="I4" s="108"/>
+      <c r="J4" s="108"/>
+      <c r="K4" s="108"/>
+      <c r="L4" s="109"/>
+      <c r="M4" s="116" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="169"/>
-      <c r="O4" s="169"/>
-      <c r="P4" s="169"/>
-      <c r="Q4" s="169"/>
-      <c r="R4" s="169"/>
-      <c r="S4" s="169"/>
-      <c r="T4" s="169"/>
-      <c r="U4" s="169"/>
-      <c r="V4" s="170"/>
-    </row>
-    <row r="5" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="163"/>
-      <c r="H5" s="163"/>
-      <c r="I5" s="163"/>
-      <c r="J5" s="163"/>
-      <c r="K5" s="163"/>
-      <c r="L5" s="164"/>
-      <c r="M5" s="179" t="s">
+      <c r="N4" s="117"/>
+      <c r="O4" s="117"/>
+      <c r="P4" s="117"/>
+      <c r="Q4" s="117"/>
+      <c r="R4" s="117"/>
+      <c r="S4" s="117"/>
+      <c r="T4" s="117"/>
+      <c r="U4" s="117"/>
+      <c r="V4" s="118"/>
+    </row>
+    <row r="5" spans="1:22" s="184" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="30"/>
+      <c r="B5" s="110"/>
+      <c r="C5" s="111"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="111"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="111"/>
+      <c r="L5" s="112"/>
+      <c r="M5" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="180"/>
-      <c r="O5" s="178"/>
+      <c r="N5" s="128"/>
+      <c r="O5" s="126"/>
       <c r="P5" s="27"/>
-      <c r="Q5" s="177" t="s">
+      <c r="Q5" s="125" t="s">
         <v>6</v>
       </c>
-      <c r="R5" s="178"/>
+      <c r="R5" s="126"/>
       <c r="S5" s="31"/>
       <c r="T5" s="27" t="s">
         <v>7</v>
@@ -3546,636 +3264,927 @@
       <c r="U5" s="26"/>
       <c r="V5" s="29"/>
     </row>
-    <row r="6" spans="2:23" s="30" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="2:23" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="146" t="s">
+    <row r="6" spans="1:22" s="184" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="30"/>
+    </row>
+    <row r="7" spans="1:22" s="184" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="30"/>
+      <c r="B7" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="122"/>
-      <c r="D7" s="122"/>
-      <c r="E7" s="147"/>
-      <c r="F7" s="147"/>
-      <c r="G7" s="147"/>
-      <c r="H7" s="147"/>
-      <c r="I7" s="147"/>
-      <c r="J7" s="147"/>
-      <c r="K7" s="147"/>
-      <c r="L7" s="122" t="s">
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="133"/>
+      <c r="F7" s="133"/>
+      <c r="G7" s="133"/>
+      <c r="H7" s="133"/>
+      <c r="I7" s="133"/>
+      <c r="J7" s="133"/>
+      <c r="K7" s="133"/>
+      <c r="L7" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="122"/>
-      <c r="N7" s="122"/>
-      <c r="O7" s="112"/>
-      <c r="P7" s="113"/>
-      <c r="Q7" s="113"/>
-      <c r="R7" s="113"/>
-      <c r="S7" s="113"/>
-      <c r="T7" s="113"/>
-      <c r="U7" s="113"/>
-      <c r="V7" s="114"/>
-    </row>
-    <row r="8" spans="2:23" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="148" t="s">
+      <c r="M7" s="86"/>
+      <c r="N7" s="86"/>
+      <c r="O7" s="78"/>
+      <c r="P7" s="79"/>
+      <c r="Q7" s="79"/>
+      <c r="R7" s="79"/>
+      <c r="S7" s="79"/>
+      <c r="T7" s="79"/>
+      <c r="U7" s="79"/>
+      <c r="V7" s="80"/>
+    </row>
+    <row r="8" spans="1:22" s="184" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="30"/>
+      <c r="B8" s="134" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="149"/>
-      <c r="D8" s="149"/>
-      <c r="E8" s="150"/>
-      <c r="F8" s="150"/>
-      <c r="G8" s="150"/>
-      <c r="H8" s="150"/>
-      <c r="I8" s="150"/>
-      <c r="J8" s="150"/>
-      <c r="K8" s="150"/>
-      <c r="L8" s="149" t="s">
+      <c r="C8" s="135"/>
+      <c r="D8" s="135"/>
+      <c r="E8" s="136"/>
+      <c r="F8" s="136"/>
+      <c r="G8" s="136"/>
+      <c r="H8" s="136"/>
+      <c r="I8" s="136"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="136"/>
+      <c r="L8" s="135" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="149"/>
-      <c r="N8" s="149"/>
-      <c r="O8" s="115"/>
-      <c r="P8" s="116"/>
-      <c r="Q8" s="116"/>
-      <c r="R8" s="116"/>
-      <c r="S8" s="116"/>
-      <c r="T8" s="116"/>
-      <c r="U8" s="116"/>
-      <c r="V8" s="117"/>
-    </row>
-    <row r="9" spans="2:23" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="148" t="s">
+      <c r="M8" s="135"/>
+      <c r="N8" s="135"/>
+      <c r="O8" s="81"/>
+      <c r="P8" s="82"/>
+      <c r="Q8" s="82"/>
+      <c r="R8" s="82"/>
+      <c r="S8" s="82"/>
+      <c r="T8" s="82"/>
+      <c r="U8" s="82"/>
+      <c r="V8" s="83"/>
+    </row>
+    <row r="9" spans="1:22" s="184" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="30"/>
+      <c r="B9" s="134" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="149"/>
-      <c r="D9" s="149"/>
-      <c r="E9" s="150"/>
-      <c r="F9" s="150"/>
-      <c r="G9" s="150"/>
-      <c r="H9" s="149" t="s">
+      <c r="C9" s="135"/>
+      <c r="D9" s="135"/>
+      <c r="E9" s="136"/>
+      <c r="F9" s="136"/>
+      <c r="G9" s="136"/>
+      <c r="H9" s="135" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="149"/>
-      <c r="J9" s="149"/>
-      <c r="K9" s="150"/>
-      <c r="L9" s="150"/>
-      <c r="M9" s="150"/>
-      <c r="N9" s="149" t="s">
+      <c r="I9" s="135"/>
+      <c r="J9" s="135"/>
+      <c r="K9" s="136"/>
+      <c r="L9" s="136"/>
+      <c r="M9" s="136"/>
+      <c r="N9" s="135" t="s">
         <v>19</v>
       </c>
-      <c r="O9" s="149"/>
-      <c r="P9" s="149"/>
-      <c r="Q9" s="149"/>
-      <c r="R9" s="149"/>
-      <c r="S9" s="149"/>
-      <c r="T9" s="150"/>
-      <c r="U9" s="150"/>
-      <c r="V9" s="184"/>
-    </row>
-    <row r="10" spans="2:23" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="151" t="s">
+      <c r="O9" s="135"/>
+      <c r="P9" s="135"/>
+      <c r="Q9" s="135"/>
+      <c r="R9" s="135"/>
+      <c r="S9" s="135"/>
+      <c r="T9" s="136"/>
+      <c r="U9" s="136"/>
+      <c r="V9" s="145"/>
+    </row>
+    <row r="10" spans="1:22" s="184" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="30"/>
+      <c r="B10" s="137" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="152"/>
-      <c r="D10" s="152"/>
-      <c r="E10" s="185"/>
-      <c r="F10" s="185"/>
-      <c r="G10" s="185"/>
-      <c r="H10" s="185"/>
-      <c r="I10" s="185"/>
-      <c r="J10" s="185"/>
-      <c r="K10" s="185"/>
-      <c r="L10" s="185"/>
-      <c r="M10" s="185"/>
-      <c r="N10" s="123" t="s">
+      <c r="C10" s="138"/>
+      <c r="D10" s="138"/>
+      <c r="E10" s="146"/>
+      <c r="F10" s="146"/>
+      <c r="G10" s="146"/>
+      <c r="H10" s="146"/>
+      <c r="I10" s="146"/>
+      <c r="J10" s="146"/>
+      <c r="K10" s="146"/>
+      <c r="L10" s="146"/>
+      <c r="M10" s="146"/>
+      <c r="N10" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="O10" s="152"/>
-      <c r="P10" s="152"/>
-      <c r="Q10" s="152"/>
-      <c r="R10" s="152"/>
-      <c r="S10" s="152"/>
-      <c r="T10" s="185"/>
-      <c r="U10" s="185"/>
-      <c r="V10" s="186"/>
-    </row>
-    <row r="11" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="N11" s="35"/>
-    </row>
-    <row r="12" spans="2:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="146" t="s">
+      <c r="O10" s="138"/>
+      <c r="P10" s="138"/>
+      <c r="Q10" s="138"/>
+      <c r="R10" s="138"/>
+      <c r="S10" s="138"/>
+      <c r="T10" s="146"/>
+      <c r="U10" s="146"/>
+      <c r="V10" s="147"/>
+    </row>
+    <row r="11" spans="1:22" s="184" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="30"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
+      <c r="S11" s="28"/>
+      <c r="T11" s="28"/>
+      <c r="U11" s="28"/>
+      <c r="V11" s="28"/>
+    </row>
+    <row r="12" spans="1:22" s="184" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="30"/>
+      <c r="B12" s="132" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="189" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="120"/>
-      <c r="E12" s="190"/>
-      <c r="F12" s="141" t="s">
+      <c r="C12" s="150" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="84"/>
+      <c r="E12" s="151"/>
+      <c r="F12" s="154" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="141" t="s">
+      <c r="G12" s="154" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="122" t="s">
+      <c r="H12" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="122"/>
-      <c r="J12" s="143" t="s">
+      <c r="I12" s="86"/>
+      <c r="J12" s="129" t="s">
         <v>25</v>
       </c>
-      <c r="K12" s="144"/>
-      <c r="L12" s="145"/>
-      <c r="M12" s="122" t="s">
+      <c r="K12" s="130"/>
+      <c r="L12" s="131"/>
+      <c r="M12" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="N12" s="120" t="s">
+      <c r="N12" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="O12" s="120"/>
-      <c r="P12" s="120"/>
-      <c r="Q12" s="128" t="s">
-        <v>75</v>
-      </c>
-      <c r="R12" s="120"/>
-      <c r="S12" s="120"/>
-      <c r="T12" s="120"/>
-      <c r="U12" s="120"/>
-      <c r="V12" s="129"/>
-      <c r="W12" s="28"/>
-    </row>
-    <row r="13" spans="2:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="151"/>
-      <c r="C13" s="191"/>
-      <c r="D13" s="121"/>
-      <c r="E13" s="192"/>
-      <c r="F13" s="142"/>
-      <c r="G13" s="142"/>
-      <c r="H13" s="152"/>
-      <c r="I13" s="152"/>
-      <c r="J13" s="193" t="s">
-        <v>77</v>
-      </c>
-      <c r="K13" s="194"/>
-      <c r="L13" s="32" t="s">
+      <c r="O12" s="84"/>
+      <c r="P12" s="84"/>
+      <c r="Q12" s="92" t="s">
+        <v>69</v>
+      </c>
+      <c r="R12" s="84"/>
+      <c r="S12" s="84"/>
+      <c r="T12" s="84"/>
+      <c r="U12" s="84"/>
+      <c r="V12" s="93"/>
+    </row>
+    <row r="13" spans="1:22" s="184" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="30"/>
+      <c r="B13" s="137"/>
+      <c r="C13" s="152"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="153"/>
+      <c r="F13" s="155"/>
+      <c r="G13" s="155"/>
+      <c r="H13" s="138"/>
+      <c r="I13" s="138"/>
+      <c r="J13" s="139" t="s">
+        <v>71</v>
+      </c>
+      <c r="K13" s="140"/>
+      <c r="L13" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="M13" s="123"/>
-      <c r="N13" s="121"/>
-      <c r="O13" s="121"/>
-      <c r="P13" s="121"/>
-      <c r="Q13" s="130"/>
-      <c r="R13" s="131"/>
-      <c r="S13" s="131"/>
-      <c r="T13" s="131"/>
-      <c r="U13" s="131"/>
-      <c r="V13" s="132"/>
-      <c r="W13" s="28"/>
-    </row>
-    <row r="14" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="36"/>
-      <c r="C14" s="188"/>
-      <c r="D14" s="124"/>
-      <c r="E14" s="125"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="187"/>
-      <c r="I14" s="187"/>
-      <c r="J14" s="195"/>
-      <c r="K14" s="196"/>
-      <c r="L14" s="197"/>
-      <c r="M14" s="33"/>
-      <c r="N14" s="124"/>
-      <c r="O14" s="124"/>
-      <c r="P14" s="125"/>
-      <c r="Q14" s="74"/>
-      <c r="R14" s="74"/>
-      <c r="S14" s="74"/>
-      <c r="T14" s="74"/>
-      <c r="U14" s="74"/>
-      <c r="V14" s="74"/>
-      <c r="W14" s="28"/>
-    </row>
-    <row r="15" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="38"/>
-      <c r="C15" s="137"/>
-      <c r="D15" s="126"/>
-      <c r="E15" s="127"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="74"/>
-      <c r="I15" s="74"/>
-      <c r="J15" s="137"/>
-      <c r="K15" s="127"/>
-      <c r="L15" s="197"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="126"/>
-      <c r="O15" s="126"/>
-      <c r="P15" s="127"/>
-      <c r="Q15" s="74"/>
-      <c r="R15" s="74"/>
-      <c r="S15" s="74"/>
-      <c r="T15" s="74"/>
-      <c r="U15" s="74"/>
-      <c r="V15" s="74"/>
-      <c r="W15" s="28"/>
-    </row>
-    <row r="16" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="38"/>
-      <c r="C16" s="137"/>
-      <c r="D16" s="126"/>
-      <c r="E16" s="127"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="74"/>
-      <c r="I16" s="74"/>
-      <c r="J16" s="137"/>
-      <c r="K16" s="127"/>
-      <c r="L16" s="197"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="126"/>
-      <c r="O16" s="126"/>
-      <c r="P16" s="127"/>
-      <c r="Q16" s="74"/>
-      <c r="R16" s="74"/>
-      <c r="S16" s="74"/>
-      <c r="T16" s="74"/>
-      <c r="U16" s="74"/>
-      <c r="V16" s="74"/>
-      <c r="W16" s="28"/>
-    </row>
-    <row r="17" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="38"/>
-      <c r="C17" s="137"/>
-      <c r="D17" s="126"/>
-      <c r="E17" s="127"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="137"/>
-      <c r="K17" s="127"/>
-      <c r="L17" s="197"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="126"/>
-      <c r="O17" s="126"/>
-      <c r="P17" s="127"/>
-      <c r="Q17" s="74"/>
-      <c r="R17" s="74"/>
-      <c r="S17" s="74"/>
-      <c r="T17" s="74"/>
-      <c r="U17" s="74"/>
-      <c r="V17" s="74"/>
-      <c r="W17" s="28"/>
-    </row>
-    <row r="18" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="38"/>
-      <c r="C18" s="115"/>
-      <c r="D18" s="116"/>
-      <c r="E18" s="136"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="74"/>
-      <c r="J18" s="137"/>
-      <c r="K18" s="127"/>
-      <c r="L18" s="197"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="126"/>
-      <c r="O18" s="126"/>
-      <c r="P18" s="127"/>
-      <c r="Q18" s="74"/>
-      <c r="R18" s="74"/>
-      <c r="S18" s="74"/>
-      <c r="T18" s="74"/>
-      <c r="U18" s="74"/>
-      <c r="V18" s="74"/>
-      <c r="W18" s="28"/>
-    </row>
-    <row r="19" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="38"/>
-      <c r="C19" s="137"/>
-      <c r="D19" s="126"/>
-      <c r="E19" s="127"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="74"/>
-      <c r="I19" s="74"/>
-      <c r="J19" s="137"/>
-      <c r="K19" s="127"/>
-      <c r="L19" s="197"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="126"/>
-      <c r="O19" s="126"/>
-      <c r="P19" s="127"/>
-      <c r="Q19" s="74"/>
-      <c r="R19" s="74"/>
-      <c r="S19" s="74"/>
-      <c r="T19" s="74"/>
-      <c r="U19" s="74"/>
-      <c r="V19" s="74"/>
-      <c r="W19" s="28"/>
-    </row>
-    <row r="20" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="38"/>
-      <c r="C20" s="137"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="127"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="137"/>
-      <c r="K20" s="127"/>
-      <c r="L20" s="197"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="126"/>
-      <c r="O20" s="126"/>
-      <c r="P20" s="127"/>
-      <c r="Q20" s="74"/>
-      <c r="R20" s="74"/>
-      <c r="S20" s="74"/>
-      <c r="T20" s="74"/>
-      <c r="U20" s="74"/>
-      <c r="V20" s="74"/>
-      <c r="W20" s="28"/>
-    </row>
-    <row r="21" spans="2:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="39"/>
-      <c r="C21" s="138"/>
-      <c r="D21" s="139"/>
-      <c r="E21" s="140"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="75"/>
-      <c r="I21" s="75"/>
-      <c r="J21" s="138"/>
-      <c r="K21" s="140"/>
-      <c r="L21" s="198"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="139"/>
-      <c r="O21" s="139"/>
-      <c r="P21" s="140"/>
-      <c r="Q21" s="75"/>
-      <c r="R21" s="75"/>
-      <c r="S21" s="75"/>
-      <c r="T21" s="75"/>
-      <c r="U21" s="75"/>
-      <c r="V21" s="75"/>
-      <c r="W21" s="28"/>
-    </row>
-    <row r="22" spans="2:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="2:23" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="133" t="s">
+      <c r="M13" s="87"/>
+      <c r="N13" s="85"/>
+      <c r="O13" s="85"/>
+      <c r="P13" s="85"/>
+      <c r="Q13" s="94"/>
+      <c r="R13" s="95"/>
+      <c r="S13" s="95"/>
+      <c r="T13" s="95"/>
+      <c r="U13" s="95"/>
+      <c r="V13" s="96"/>
+    </row>
+    <row r="14" spans="1:22" s="184" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="30"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="149"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="148"/>
+      <c r="I14" s="148"/>
+      <c r="J14" s="141"/>
+      <c r="K14" s="142"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="88"/>
+      <c r="O14" s="88"/>
+      <c r="P14" s="89"/>
+      <c r="Q14" s="97"/>
+      <c r="R14" s="97"/>
+      <c r="S14" s="97"/>
+      <c r="T14" s="97"/>
+      <c r="U14" s="97"/>
+      <c r="V14" s="98"/>
+    </row>
+    <row r="15" spans="1:22" s="184" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="30"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="143"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="97"/>
+      <c r="I15" s="97"/>
+      <c r="J15" s="143"/>
+      <c r="K15" s="91"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="90"/>
+      <c r="O15" s="90"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="97"/>
+      <c r="R15" s="97"/>
+      <c r="S15" s="97"/>
+      <c r="T15" s="97"/>
+      <c r="U15" s="97"/>
+      <c r="V15" s="98"/>
+    </row>
+    <row r="16" spans="1:22" s="184" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="30"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="143"/>
+      <c r="D16" s="90"/>
+      <c r="E16" s="91"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="97"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="143"/>
+      <c r="K16" s="91"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="90"/>
+      <c r="O16" s="90"/>
+      <c r="P16" s="91"/>
+      <c r="Q16" s="97"/>
+      <c r="R16" s="97"/>
+      <c r="S16" s="97"/>
+      <c r="T16" s="97"/>
+      <c r="U16" s="97"/>
+      <c r="V16" s="98"/>
+    </row>
+    <row r="17" spans="1:23" s="184" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="30"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="143"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="91"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="97"/>
+      <c r="I17" s="97"/>
+      <c r="J17" s="143"/>
+      <c r="K17" s="91"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="90"/>
+      <c r="O17" s="90"/>
+      <c r="P17" s="91"/>
+      <c r="Q17" s="97"/>
+      <c r="R17" s="97"/>
+      <c r="S17" s="97"/>
+      <c r="T17" s="97"/>
+      <c r="U17" s="97"/>
+      <c r="V17" s="98"/>
+    </row>
+    <row r="18" spans="1:23" s="184" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="30"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="169"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="97"/>
+      <c r="I18" s="97"/>
+      <c r="J18" s="143"/>
+      <c r="K18" s="91"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="90"/>
+      <c r="O18" s="90"/>
+      <c r="P18" s="91"/>
+      <c r="Q18" s="97"/>
+      <c r="R18" s="97"/>
+      <c r="S18" s="97"/>
+      <c r="T18" s="97"/>
+      <c r="U18" s="97"/>
+      <c r="V18" s="98"/>
+    </row>
+    <row r="19" spans="1:23" s="184" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="30"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="143"/>
+      <c r="D19" s="90"/>
+      <c r="E19" s="91"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="97"/>
+      <c r="I19" s="97"/>
+      <c r="J19" s="143"/>
+      <c r="K19" s="91"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="90"/>
+      <c r="O19" s="90"/>
+      <c r="P19" s="91"/>
+      <c r="Q19" s="97"/>
+      <c r="R19" s="97"/>
+      <c r="S19" s="97"/>
+      <c r="T19" s="97"/>
+      <c r="U19" s="97"/>
+      <c r="V19" s="98"/>
+    </row>
+    <row r="20" spans="1:23" s="184" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="30"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="143"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="91"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="97"/>
+      <c r="I20" s="97"/>
+      <c r="J20" s="143"/>
+      <c r="K20" s="91"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="90"/>
+      <c r="O20" s="90"/>
+      <c r="P20" s="91"/>
+      <c r="Q20" s="97"/>
+      <c r="R20" s="97"/>
+      <c r="S20" s="97"/>
+      <c r="T20" s="97"/>
+      <c r="U20" s="97"/>
+      <c r="V20" s="98"/>
+    </row>
+    <row r="21" spans="1:23" s="184" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="30"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="170"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="99"/>
+      <c r="I21" s="99"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="77"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="170"/>
+      <c r="O21" s="170"/>
+      <c r="P21" s="77"/>
+      <c r="Q21" s="99"/>
+      <c r="R21" s="99"/>
+      <c r="S21" s="99"/>
+      <c r="T21" s="99"/>
+      <c r="U21" s="99"/>
+      <c r="V21" s="100"/>
+    </row>
+    <row r="22" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="183"/>
+      <c r="B22" s="183"/>
+      <c r="C22" s="183"/>
+      <c r="D22" s="183"/>
+      <c r="E22" s="183"/>
+      <c r="F22" s="183"/>
+      <c r="G22" s="183"/>
+      <c r="H22" s="183"/>
+      <c r="I22" s="183"/>
+      <c r="J22" s="183"/>
+      <c r="K22" s="183"/>
+      <c r="L22" s="183"/>
+      <c r="M22" s="183"/>
+      <c r="N22" s="183"/>
+      <c r="O22" s="183"/>
+      <c r="P22" s="183"/>
+      <c r="Q22" s="183"/>
+      <c r="R22" s="183"/>
+      <c r="S22" s="183"/>
+      <c r="T22" s="183"/>
+      <c r="U22" s="183"/>
+      <c r="V22" s="183"/>
+      <c r="W22" s="183"/>
+    </row>
+    <row r="23" spans="1:23" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="166" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="134"/>
-      <c r="D23" s="134"/>
-      <c r="E23" s="134"/>
-      <c r="F23" s="134"/>
-      <c r="G23" s="134"/>
-      <c r="H23" s="134"/>
-      <c r="I23" s="134"/>
-      <c r="J23" s="134"/>
-      <c r="K23" s="134"/>
-      <c r="L23" s="134"/>
-      <c r="M23" s="134"/>
-      <c r="N23" s="134"/>
-      <c r="O23" s="134"/>
-      <c r="P23" s="134"/>
-      <c r="Q23" s="134"/>
-      <c r="R23" s="134"/>
-      <c r="S23" s="134"/>
-      <c r="T23" s="134"/>
-      <c r="U23" s="134"/>
-      <c r="V23" s="135"/>
-    </row>
-    <row r="24" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="105" t="s">
+      <c r="C23" s="167"/>
+      <c r="D23" s="167"/>
+      <c r="E23" s="167"/>
+      <c r="F23" s="167"/>
+      <c r="G23" s="167"/>
+      <c r="H23" s="167"/>
+      <c r="I23" s="167"/>
+      <c r="J23" s="167"/>
+      <c r="K23" s="167"/>
+      <c r="L23" s="167"/>
+      <c r="M23" s="167"/>
+      <c r="N23" s="167"/>
+      <c r="O23" s="167"/>
+      <c r="P23" s="167"/>
+      <c r="Q23" s="167"/>
+      <c r="R23" s="167"/>
+      <c r="S23" s="167"/>
+      <c r="T23" s="167"/>
+      <c r="U23" s="167"/>
+      <c r="V23" s="168"/>
+    </row>
+    <row r="24" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="184"/>
+      <c r="B24" s="184"/>
+      <c r="C24" s="184"/>
+      <c r="D24" s="184"/>
+      <c r="E24" s="184"/>
+      <c r="F24" s="184"/>
+      <c r="G24" s="184"/>
+      <c r="H24" s="184"/>
+      <c r="I24" s="184"/>
+      <c r="J24" s="184"/>
+      <c r="K24" s="184"/>
+      <c r="L24" s="184"/>
+      <c r="M24" s="184"/>
+      <c r="N24" s="184"/>
+      <c r="O24" s="184"/>
+      <c r="P24" s="184"/>
+      <c r="Q24" s="184"/>
+      <c r="R24" s="184"/>
+      <c r="S24" s="184"/>
+      <c r="T24" s="184"/>
+      <c r="U24" s="184"/>
+      <c r="V24" s="184"/>
+    </row>
+    <row r="25" spans="1:23" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="174" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="175"/>
+      <c r="D25" s="175"/>
+      <c r="E25" s="175"/>
+      <c r="F25" s="175"/>
+      <c r="G25" s="175"/>
+      <c r="H25" s="175"/>
+      <c r="I25" s="175"/>
+      <c r="J25" s="175"/>
+      <c r="K25" s="175"/>
+      <c r="L25" s="175"/>
+      <c r="M25" s="175"/>
+      <c r="N25" s="175"/>
+      <c r="O25" s="175"/>
+      <c r="P25" s="175"/>
+      <c r="Q25" s="175"/>
+      <c r="R25" s="175"/>
+      <c r="S25" s="175"/>
+      <c r="T25" s="175"/>
+      <c r="U25" s="175"/>
+      <c r="V25" s="176"/>
+    </row>
+    <row r="26" spans="1:23" ht="27.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="144"/>
+      <c r="C26" s="144"/>
+      <c r="D26" s="144"/>
+      <c r="E26" s="144"/>
+      <c r="F26" s="144"/>
+      <c r="G26" s="144"/>
+      <c r="H26" s="144"/>
+      <c r="I26" s="144"/>
+      <c r="J26" s="144"/>
+      <c r="K26" s="144"/>
+      <c r="L26" s="144"/>
+      <c r="M26" s="144"/>
+      <c r="N26" s="144"/>
+      <c r="O26" s="144"/>
+      <c r="P26" s="144"/>
+      <c r="Q26" s="144"/>
+      <c r="R26" s="144"/>
+      <c r="S26" s="144"/>
+      <c r="T26" s="144"/>
+      <c r="U26" s="144"/>
+      <c r="V26" s="144"/>
+    </row>
+    <row r="27" spans="1:23" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="156" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="105"/>
-      <c r="D25" s="105"/>
-      <c r="E25" s="105"/>
-      <c r="F25" s="105"/>
-      <c r="G25" s="106"/>
-      <c r="H25" s="107" t="s">
+      <c r="C27" s="157"/>
+      <c r="D27" s="157"/>
+      <c r="E27" s="157"/>
+      <c r="F27" s="157"/>
+      <c r="G27" s="158"/>
+      <c r="H27" s="159" t="s">
         <v>49</v>
       </c>
-      <c r="I25" s="108"/>
-      <c r="J25" s="108"/>
-      <c r="K25" s="108"/>
-      <c r="L25" s="108"/>
-      <c r="M25" s="109"/>
-      <c r="N25" s="107" t="s">
+      <c r="I27" s="160"/>
+      <c r="J27" s="160"/>
+      <c r="K27" s="160"/>
+      <c r="L27" s="160"/>
+      <c r="M27" s="161"/>
+      <c r="N27" s="159" t="s">
         <v>50</v>
       </c>
-      <c r="O25" s="108"/>
-      <c r="P25" s="108"/>
-      <c r="Q25" s="108"/>
-      <c r="R25" s="108"/>
-      <c r="S25" s="108"/>
-      <c r="T25" s="108"/>
-      <c r="U25" s="108"/>
-      <c r="V25" s="109"/>
-    </row>
-    <row r="26" spans="2:23" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="110" t="s">
+      <c r="O27" s="160"/>
+      <c r="P27" s="160"/>
+      <c r="Q27" s="160"/>
+      <c r="R27" s="160"/>
+      <c r="S27" s="160"/>
+      <c r="T27" s="160"/>
+      <c r="U27" s="160"/>
+      <c r="V27" s="161"/>
+    </row>
+    <row r="28" spans="1:23" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="162" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="111"/>
-      <c r="D26" s="91"/>
-      <c r="E26" s="91"/>
-      <c r="F26" s="91"/>
-      <c r="G26" s="92"/>
-      <c r="H26" s="87" t="s">
+      <c r="C28" s="163"/>
+      <c r="D28" s="181"/>
+      <c r="E28" s="181"/>
+      <c r="F28" s="181"/>
+      <c r="G28" s="141"/>
+      <c r="H28" s="164" t="s">
         <v>51</v>
       </c>
-      <c r="I26" s="88"/>
-      <c r="J26" s="102"/>
-      <c r="K26" s="102"/>
-      <c r="L26" s="102"/>
-      <c r="M26" s="103"/>
-      <c r="N26" s="87" t="s">
+      <c r="I28" s="165"/>
+      <c r="J28" s="97"/>
+      <c r="K28" s="97"/>
+      <c r="L28" s="97"/>
+      <c r="M28" s="98"/>
+      <c r="N28" s="164" t="s">
         <v>51</v>
       </c>
-      <c r="O26" s="88"/>
-      <c r="P26" s="88"/>
-      <c r="Q26" s="74"/>
-      <c r="R26" s="74"/>
-      <c r="S26" s="74"/>
-      <c r="T26" s="74"/>
-      <c r="U26" s="74"/>
-      <c r="V26" s="118"/>
-    </row>
-    <row r="27" spans="2:23" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="89" t="s">
+      <c r="O28" s="165"/>
+      <c r="P28" s="165"/>
+      <c r="Q28" s="97"/>
+      <c r="R28" s="97"/>
+      <c r="S28" s="97"/>
+      <c r="T28" s="97"/>
+      <c r="U28" s="97"/>
+      <c r="V28" s="98"/>
+    </row>
+    <row r="29" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="179" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="90"/>
-      <c r="D27" s="93"/>
-      <c r="E27" s="93"/>
-      <c r="F27" s="93"/>
-      <c r="G27" s="94"/>
-      <c r="H27" s="89" t="s">
+      <c r="C29" s="180"/>
+      <c r="D29" s="99"/>
+      <c r="E29" s="99"/>
+      <c r="F29" s="99"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="179" t="s">
         <v>52</v>
       </c>
-      <c r="I27" s="90"/>
-      <c r="J27" s="93"/>
-      <c r="K27" s="93"/>
-      <c r="L27" s="93"/>
-      <c r="M27" s="104"/>
-      <c r="N27" s="89" t="s">
+      <c r="I29" s="180"/>
+      <c r="J29" s="99"/>
+      <c r="K29" s="99"/>
+      <c r="L29" s="99"/>
+      <c r="M29" s="100"/>
+      <c r="N29" s="179" t="s">
         <v>52</v>
       </c>
-      <c r="O27" s="90"/>
-      <c r="P27" s="90"/>
-      <c r="Q27" s="75"/>
-      <c r="R27" s="75"/>
-      <c r="S27" s="75"/>
-      <c r="T27" s="75"/>
-      <c r="U27" s="75"/>
-      <c r="V27" s="119"/>
-    </row>
-    <row r="28" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="79" t="s">
+      <c r="O29" s="180"/>
+      <c r="P29" s="180"/>
+      <c r="Q29" s="99"/>
+      <c r="R29" s="99"/>
+      <c r="S29" s="99"/>
+      <c r="T29" s="99"/>
+      <c r="U29" s="99"/>
+      <c r="V29" s="100"/>
+    </row>
+    <row r="30" spans="1:23" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="184"/>
+      <c r="B30" s="184"/>
+      <c r="C30" s="184"/>
+      <c r="D30" s="184"/>
+      <c r="E30" s="184"/>
+      <c r="F30" s="184"/>
+      <c r="G30" s="184"/>
+      <c r="H30" s="184"/>
+      <c r="I30" s="184"/>
+      <c r="J30" s="184"/>
+      <c r="K30" s="184"/>
+      <c r="L30" s="184"/>
+      <c r="M30" s="184"/>
+      <c r="N30" s="184"/>
+      <c r="O30" s="184"/>
+      <c r="P30" s="184"/>
+      <c r="Q30" s="184"/>
+      <c r="R30" s="184"/>
+      <c r="S30" s="184"/>
+      <c r="T30" s="184"/>
+      <c r="U30" s="184"/>
+      <c r="V30" s="184"/>
+    </row>
+    <row r="31" spans="1:23" ht="27.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:23" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:23" ht="30.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="1:23" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="1:23" ht="33.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:23" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="92" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="84"/>
+      <c r="D37" s="84"/>
+      <c r="E37" s="84"/>
+      <c r="F37" s="84"/>
+      <c r="G37" s="84"/>
+      <c r="H37" s="84"/>
+      <c r="I37" s="84"/>
+      <c r="J37" s="84"/>
+      <c r="K37" s="93"/>
+      <c r="L37" s="92" t="s">
+        <v>73</v>
+      </c>
+      <c r="M37" s="84"/>
+      <c r="N37" s="84"/>
+      <c r="O37" s="84"/>
+      <c r="P37" s="84"/>
+      <c r="Q37" s="84"/>
+      <c r="R37" s="84"/>
+      <c r="S37" s="84"/>
+      <c r="T37" s="84"/>
+      <c r="U37" s="84"/>
+      <c r="V37" s="93"/>
+    </row>
+    <row r="38" spans="1:23" ht="33.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="177"/>
+      <c r="C38" s="85"/>
+      <c r="D38" s="85"/>
+      <c r="E38" s="85"/>
+      <c r="F38" s="85"/>
+      <c r="G38" s="85"/>
+      <c r="H38" s="85"/>
+      <c r="I38" s="85"/>
+      <c r="J38" s="85"/>
+      <c r="K38" s="178"/>
+      <c r="L38" s="177"/>
+      <c r="M38" s="85"/>
+      <c r="N38" s="85"/>
+      <c r="O38" s="85"/>
+      <c r="P38" s="85"/>
+      <c r="Q38" s="85"/>
+      <c r="R38" s="85"/>
+      <c r="S38" s="85"/>
+      <c r="T38" s="85"/>
+      <c r="U38" s="85"/>
+      <c r="V38" s="178"/>
+    </row>
+    <row r="39" spans="1:23" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="171"/>
+      <c r="C39" s="172"/>
+      <c r="D39" s="172"/>
+      <c r="E39" s="172"/>
+      <c r="F39" s="172"/>
+      <c r="G39" s="172"/>
+      <c r="H39" s="172"/>
+      <c r="I39" s="172"/>
+      <c r="J39" s="172"/>
+      <c r="K39" s="173"/>
+      <c r="L39" s="171"/>
+      <c r="M39" s="172"/>
+      <c r="N39" s="172"/>
+      <c r="O39" s="172"/>
+      <c r="P39" s="172"/>
+      <c r="Q39" s="172"/>
+      <c r="R39" s="172"/>
+      <c r="S39" s="172"/>
+      <c r="T39" s="172"/>
+      <c r="U39" s="172"/>
+      <c r="V39" s="173"/>
+    </row>
+    <row r="40" spans="1:23" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="188"/>
+      <c r="C40" s="188"/>
+      <c r="D40" s="188"/>
+      <c r="E40" s="188"/>
+      <c r="F40" s="188"/>
+      <c r="G40" s="188"/>
+      <c r="H40" s="188"/>
+      <c r="I40" s="188"/>
+      <c r="J40" s="188"/>
+      <c r="K40" s="188"/>
+      <c r="L40" s="188"/>
+      <c r="M40" s="188"/>
+      <c r="N40" s="188"/>
+      <c r="O40" s="188"/>
+      <c r="P40" s="188"/>
+      <c r="Q40" s="188"/>
+      <c r="R40" s="188"/>
+      <c r="S40" s="188"/>
+      <c r="T40" s="188"/>
+      <c r="U40" s="188"/>
+      <c r="V40" s="188"/>
+    </row>
+    <row r="41" spans="1:23" ht="98.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="185" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="80"/>
-      <c r="D29" s="80"/>
-      <c r="E29" s="80"/>
-      <c r="F29" s="80"/>
-      <c r="G29" s="81"/>
-      <c r="H29" s="95" t="s">
-        <v>54</v>
-      </c>
-      <c r="I29" s="96"/>
-      <c r="J29" s="96"/>
-      <c r="K29" s="96"/>
-      <c r="L29" s="96"/>
-      <c r="M29" s="96"/>
-      <c r="N29" s="96"/>
-      <c r="O29" s="96"/>
-      <c r="P29" s="96"/>
-      <c r="Q29" s="96"/>
-      <c r="R29" s="96"/>
-      <c r="S29" s="96"/>
-      <c r="T29" s="96"/>
-      <c r="U29" s="96"/>
-      <c r="V29" s="97"/>
-    </row>
-    <row r="30" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="82"/>
-      <c r="C30" s="83"/>
-      <c r="D30" s="83"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="83"/>
-      <c r="G30" s="84"/>
-      <c r="H30" s="85" t="s">
-        <v>55</v>
-      </c>
-      <c r="I30" s="86"/>
-      <c r="J30" s="86" t="s">
-        <v>56</v>
-      </c>
-      <c r="K30" s="86"/>
-      <c r="L30" s="86" t="s">
-        <v>57</v>
-      </c>
-      <c r="M30" s="86"/>
-      <c r="N30" s="86"/>
-      <c r="O30" s="86"/>
-      <c r="P30" s="86" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q30" s="86"/>
-      <c r="R30" s="86"/>
-      <c r="S30" s="86"/>
-      <c r="T30" s="86"/>
-      <c r="U30" s="86"/>
-      <c r="V30" s="98"/>
-    </row>
-    <row r="31" spans="2:23" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="76"/>
-      <c r="C31" s="77"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="101"/>
-      <c r="I31" s="99"/>
-      <c r="J31" s="99"/>
-      <c r="K31" s="99"/>
-      <c r="L31" s="99"/>
-      <c r="M31" s="99"/>
-      <c r="N31" s="99"/>
-      <c r="O31" s="99"/>
-      <c r="P31" s="99"/>
-      <c r="Q31" s="99"/>
-      <c r="R31" s="99"/>
-      <c r="S31" s="99"/>
-      <c r="T31" s="99"/>
-      <c r="U31" s="99"/>
-      <c r="V31" s="100"/>
-    </row>
-    <row r="32" spans="2:23" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="183"/>
-      <c r="C32" s="183"/>
-      <c r="D32" s="183"/>
-      <c r="E32" s="183"/>
-      <c r="F32" s="183"/>
-      <c r="G32" s="183"/>
-      <c r="H32" s="183"/>
-      <c r="I32" s="183"/>
-      <c r="J32" s="183"/>
-      <c r="K32" s="183"/>
-      <c r="L32" s="183"/>
-      <c r="M32" s="183"/>
-      <c r="N32" s="183"/>
-      <c r="O32" s="183"/>
-      <c r="P32" s="183"/>
-      <c r="Q32" s="183"/>
-      <c r="R32" s="183"/>
-      <c r="S32" s="183"/>
-      <c r="T32" s="183"/>
-      <c r="U32" s="183"/>
-      <c r="V32" s="183"/>
-    </row>
-    <row r="33" spans="2:22" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="181" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="182"/>
-      <c r="D33" s="182"/>
-      <c r="E33" s="182"/>
-      <c r="F33" s="182"/>
-      <c r="G33" s="182"/>
-      <c r="H33" s="182"/>
-      <c r="I33" s="182"/>
-      <c r="J33" s="182"/>
-      <c r="K33" s="182"/>
-      <c r="L33" s="182"/>
-      <c r="M33" s="182"/>
-      <c r="N33" s="182"/>
-      <c r="O33" s="182"/>
-      <c r="P33" s="182"/>
-      <c r="Q33" s="182"/>
-      <c r="R33" s="182"/>
-      <c r="S33" s="182"/>
-      <c r="T33" s="182"/>
-      <c r="U33" s="182"/>
-      <c r="V33" s="182"/>
-    </row>
-    <row r="34" spans="2:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="2:22" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="2:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="2:22" ht="109.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.3"/>
+      <c r="C41" s="186"/>
+      <c r="D41" s="186"/>
+      <c r="E41" s="186"/>
+      <c r="F41" s="186"/>
+      <c r="G41" s="186"/>
+      <c r="H41" s="186"/>
+      <c r="I41" s="186"/>
+      <c r="J41" s="186"/>
+      <c r="K41" s="186"/>
+      <c r="L41" s="186"/>
+      <c r="M41" s="186"/>
+      <c r="N41" s="186"/>
+      <c r="O41" s="186"/>
+      <c r="P41" s="186"/>
+      <c r="Q41" s="186"/>
+      <c r="R41" s="186"/>
+      <c r="S41" s="186"/>
+      <c r="T41" s="186"/>
+      <c r="U41" s="186"/>
+      <c r="V41" s="187"/>
+    </row>
+    <row r="42" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="182"/>
+      <c r="B42" s="183"/>
+      <c r="C42" s="183"/>
+      <c r="D42" s="183"/>
+      <c r="E42" s="183"/>
+      <c r="F42" s="183"/>
+      <c r="G42" s="183"/>
+      <c r="H42" s="183"/>
+      <c r="I42" s="183"/>
+      <c r="J42" s="183"/>
+      <c r="K42" s="183"/>
+      <c r="L42" s="183"/>
+      <c r="M42" s="183"/>
+      <c r="N42" s="183"/>
+      <c r="O42" s="183"/>
+      <c r="P42" s="183"/>
+      <c r="Q42" s="183"/>
+      <c r="R42" s="183"/>
+      <c r="S42" s="183"/>
+      <c r="T42" s="183"/>
+      <c r="U42" s="183"/>
+      <c r="V42" s="183"/>
+      <c r="W42" s="182"/>
+    </row>
+    <row r="43" spans="1:23" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:23" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:23" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:23" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:23" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:23" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="201" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="202" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="203" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="204" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="205" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="206" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="207" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="208" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="209" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="210" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="211" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="212" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="213" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="214" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="215" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="216" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="217" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="218" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="219" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="220" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="221" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="222" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="223" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="224" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="225" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="226" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="227" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="228" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="229" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="230" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="231" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="232" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="233" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="234" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="235" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="236" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="237" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="238" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1161" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1162" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1163" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1164" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1165" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1166" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1167" ht="148.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="105">
-    <mergeCell ref="B33:V33"/>
-    <mergeCell ref="B32:V32"/>
+    <mergeCell ref="B42:V42"/>
+    <mergeCell ref="A22:W22"/>
+    <mergeCell ref="A24:V24"/>
+    <mergeCell ref="W1:XFD21"/>
+    <mergeCell ref="A30:V30"/>
+    <mergeCell ref="B40:V40"/>
+    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="L39:V39"/>
+    <mergeCell ref="Q29:V29"/>
+    <mergeCell ref="B25:V25"/>
+    <mergeCell ref="B37:K38"/>
+    <mergeCell ref="L37:V38"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="B23:V23"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="N27:V27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="Q28:V28"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B41:V41"/>
+    <mergeCell ref="B26:V26"/>
     <mergeCell ref="T9:V9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="N10:S10"/>
@@ -4190,14 +4199,8 @@
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="J12:L12"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="E7:K7"/>
     <mergeCell ref="L7:N7"/>
@@ -4206,6 +4209,12 @@
     <mergeCell ref="L8:N8"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="H12:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
     <mergeCell ref="E2:L3"/>
     <mergeCell ref="B4:L5"/>
     <mergeCell ref="M2:V2"/>
@@ -4214,33 +4223,9 @@
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="Q5:R5"/>
     <mergeCell ref="M5:O5"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J21:K21"/>
     <mergeCell ref="O7:V7"/>
     <mergeCell ref="O8:V8"/>
-    <mergeCell ref="N25:V25"/>
-    <mergeCell ref="Q26:V26"/>
-    <mergeCell ref="Q27:V27"/>
     <mergeCell ref="N12:P13"/>
     <mergeCell ref="M12:M13"/>
     <mergeCell ref="N14:P14"/>
@@ -4248,93 +4233,17 @@
     <mergeCell ref="Q12:V13"/>
     <mergeCell ref="Q15:V15"/>
     <mergeCell ref="Q14:V14"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B23:V23"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
     <mergeCell ref="Q16:V16"/>
     <mergeCell ref="Q17:V17"/>
     <mergeCell ref="Q18:V18"/>
     <mergeCell ref="Q19:V19"/>
     <mergeCell ref="Q20:V20"/>
     <mergeCell ref="Q21:V21"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B29:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="H29:V29"/>
-    <mergeCell ref="P30:V30"/>
-    <mergeCell ref="P31:V31"/>
-    <mergeCell ref="L30:O30"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:O31"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="B25:G25"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="56" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2050" r:id="rId4" name="Check Box 2">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>19</xdr:col>
-                    <xdr:colOff>352425</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>20</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>438150</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2051" r:id="rId5" name="Check Box 3">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>20</xdr:col>
-                    <xdr:colOff>238125</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>38100</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>22</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>438150</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-  </mc:AlternateContent>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -4373,13 +4282,13 @@
   <sheetData>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -4387,32 +4296,32 @@
         <v>18</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -4422,22 +4331,22 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D9" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D10" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D11" s="5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D12" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -4763,16 +4672,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9354BF11-9FAB-41DC-AD6D-CC1A4CAFF506}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="446f4af2-8620-4618-9f40-d116a642c3b9"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="3f38b58c-1ade-4b62-bc3e-d0a84c2c5900"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
cambios ya casi finales profavorrr
</commit_message>
<xml_diff>
--- a/templates/plantilla.xlsx
+++ b/templates/plantilla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\Requisiciones\camunda_back\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E0B1F0-8802-4AA5-BEE7-15336D10747F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFC90EB-C61D-4E28-A097-312B5C3DB243}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{6CC2AB2B-0F37-47AE-B363-6A70476DA6B2}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" firstSheet="1" activeTab="1" xr2:uid="{6CC2AB2B-0F37-47AE-B363-6A70476DA6B2}"/>
   </bookViews>
   <sheets>
     <sheet name="FORMATO" sheetId="3" state="hidden" r:id="rId1"/>
@@ -24,17 +24,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -347,7 +336,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-[$$-240A]\ * #,##0.00_-;\-[$$-240A]\ * #,##0.00_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
@@ -1169,9 +1158,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1257,6 +1246,30 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1377,28 +1390,169 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1410,160 +1564,55 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1572,6 +1621,12 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1583,9 +1638,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1610,72 +1662,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1695,14 +1681,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1725,7 +1703,7 @@
         <xdr:cNvPr id="2" name="Imagen 1" descr="logo COOPIDROGAS con texto">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{576A7ADA-E932-4693-89D7-6ADAF7F47644}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1785,7 +1763,7 @@
         <xdr:cNvPr id="3" name="Imagen 2" descr="logo COOPIDROGAS con texto">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{941A4DAC-45F7-46B9-AB93-C72F1EBEDDF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1840,7 +1818,7 @@
         <xdr:cNvPr id="4" name="CuadroTexto 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02BB6DC2-493A-41EA-F949-3A704375F2B1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1880,12 +1858,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100">
-              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>SI</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-CO" sz="1100">
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1909,7 +1884,7 @@
         <xdr:cNvPr id="5" name="CuadroTexto 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{084F8564-AF65-4983-A2E4-1EC94CFF5C85}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1949,158 +1924,21 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100">
-              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>NO</a:t>
-          </a:r>
+          <a:endParaRPr lang="es-CO" sz="1100">
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>19</xdr:col>
-          <xdr:colOff>350520</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>45720</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>20</xdr:col>
-          <xdr:colOff>106680</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>441960</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2050" name="Check Box 2" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2050"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>20</xdr:col>
-          <xdr:colOff>236220</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>21</xdr:col>
-          <xdr:colOff>416202</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>441960</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2051" name="Check Box 3" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2051"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003080000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2138,7 +1976,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2244,7 +2082,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2386,7 +2224,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2400,22 +2238,22 @@
       <selection activeCell="C12" sqref="C12:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" customWidth="1"/>
-    <col min="2" max="2" width="0.88671875" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="0.85546875" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="29.109375" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
     <col min="8" max="9" width="5" customWidth="1"/>
-    <col min="10" max="10" width="30.109375" customWidth="1"/>
-    <col min="11" max="16" width="7.5546875" customWidth="1"/>
-    <col min="17" max="17" width="1.5546875" customWidth="1"/>
+    <col min="10" max="10" width="30.140625" customWidth="1"/>
+    <col min="11" max="16" width="7.5703125" customWidth="1"/>
+    <col min="17" max="17" width="1.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:17" ht="4.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:17" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:17" ht="4.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" s="8"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -2433,80 +2271,80 @@
       <c r="P2" s="9"/>
       <c r="Q2" s="10"/>
     </row>
-    <row r="3" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="53" t="s">
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53" t="s">
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
       <c r="Q3" s="12"/>
     </row>
-    <row r="4" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="11"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53" t="s">
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="53"/>
-      <c r="M4" s="53"/>
-      <c r="N4" s="53"/>
-      <c r="O4" s="53"/>
-      <c r="P4" s="53"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
       <c r="Q4" s="12"/>
     </row>
-    <row r="5" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="11"/>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="54" t="s">
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="54"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="54"/>
-      <c r="O5" s="54"/>
-      <c r="P5" s="54"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="62"/>
       <c r="Q5" s="12"/>
     </row>
-    <row r="6" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="48"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="56"/>
       <c r="K6" s="3" t="s">
         <v>11</v>
       </c>
@@ -2521,32 +2359,32 @@
       <c r="P6" s="3"/>
       <c r="Q6" s="12"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="11"/>
       <c r="Q7" s="12"/>
     </row>
-    <row r="8" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="11"/>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="I8" s="41" t="s">
+      <c r="D8" s="58"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="I8" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="41"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="42"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="50"/>
       <c r="Q8" s="12"/>
     </row>
-    <row r="9" spans="2:17" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:17" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="11"/>
       <c r="C9" s="13"/>
       <c r="J9" s="13"/>
@@ -2555,12 +2393,12 @@
       <c r="M9" s="14"/>
       <c r="Q9" s="12"/>
     </row>
-    <row r="10" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="11"/>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="50"/>
+      <c r="D10" s="58"/>
       <c r="E10" s="24"/>
       <c r="F10" s="15" t="s">
         <v>28</v>
@@ -2568,11 +2406,11 @@
       <c r="G10" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="41" t="s">
+      <c r="H10" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
       <c r="K10" s="16" t="s">
         <v>2</v>
       </c>
@@ -2583,141 +2421,141 @@
       <c r="N10" s="5"/>
       <c r="Q10" s="12"/>
     </row>
-    <row r="11" spans="2:17" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:17" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="11"/>
       <c r="C11" s="13"/>
       <c r="Q11" s="12"/>
     </row>
-    <row r="12" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="11"/>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="50"/>
+      <c r="D12" s="58"/>
       <c r="E12" s="24"/>
-      <c r="F12" s="41" t="s">
+      <c r="F12" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="41"/>
-      <c r="H12" s="42" t="s">
+      <c r="G12" s="49"/>
+      <c r="H12" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="42"/>
-      <c r="J12" s="41" t="s">
+      <c r="I12" s="50"/>
+      <c r="J12" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="42" t="str">
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="50" t="str">
         <f>VLOOKUP(H12,Hoja3!B4:C7,2,FALSE)</f>
         <v>HASTA 5 DÍAS HÁBILES</v>
       </c>
-      <c r="N12" s="42"/>
-      <c r="O12" s="42"/>
-      <c r="P12" s="42"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
       <c r="Q12" s="12"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="11"/>
       <c r="Q13" s="12"/>
     </row>
-    <row r="14" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11"/>
-      <c r="C14" s="72" t="s">
+      <c r="C14" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
-      <c r="K14" s="72"/>
-      <c r="L14" s="72"/>
-      <c r="M14" s="72"/>
-      <c r="N14" s="72"/>
-      <c r="O14" s="72"/>
-      <c r="P14" s="72"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="80"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="80"/>
+      <c r="N14" s="80"/>
+      <c r="O14" s="80"/>
+      <c r="P14" s="80"/>
       <c r="Q14" s="12"/>
     </row>
-    <row r="15" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="11"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="56"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="56"/>
-      <c r="O15" s="56"/>
-      <c r="P15" s="56"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="64"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="64"/>
+      <c r="N15" s="64"/>
+      <c r="O15" s="64"/>
+      <c r="P15" s="64"/>
       <c r="Q15" s="12"/>
     </row>
-    <row r="16" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="11"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="56"/>
-      <c r="P16" s="56"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="64"/>
+      <c r="M16" s="64"/>
+      <c r="N16" s="64"/>
+      <c r="O16" s="64"/>
+      <c r="P16" s="64"/>
       <c r="Q16" s="12"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="11"/>
       <c r="Q17" s="12"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="11"/>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="49" t="s">
+      <c r="D18" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49" t="s">
+      <c r="E18" s="57"/>
+      <c r="F18" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="49" t="s">
+      <c r="G18" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="49" t="s">
+      <c r="H18" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
-      <c r="K18" s="49" t="s">
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="L18" s="49"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="49"/>
-      <c r="P18" s="49"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="57"/>
+      <c r="P18" s="57"/>
       <c r="Q18" s="12"/>
     </row>
-    <row r="19" spans="2:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="11"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
       <c r="H19" s="1" t="s">
         <v>2</v>
       </c>
@@ -2727,424 +2565,424 @@
       <c r="J19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K19" s="49"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="49"/>
-      <c r="N19" s="49"/>
-      <c r="O19" s="49"/>
-      <c r="P19" s="49"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="57"/>
+      <c r="N19" s="57"/>
+      <c r="O19" s="57"/>
+      <c r="P19" s="57"/>
       <c r="Q19" s="12"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="11"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="40"/>
-      <c r="O20" s="40"/>
-      <c r="P20" s="40"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="48"/>
       <c r="Q20" s="12"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="11"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="40"/>
-      <c r="L21" s="40"/>
-      <c r="M21" s="40"/>
-      <c r="N21" s="40"/>
-      <c r="O21" s="40"/>
-      <c r="P21" s="40"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
+      <c r="P21" s="48"/>
       <c r="Q21" s="12"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="40"/>
-      <c r="O22" s="40"/>
-      <c r="P22" s="40"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="48"/>
       <c r="Q22" s="12"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="40"/>
-      <c r="N23" s="40"/>
-      <c r="O23" s="40"/>
-      <c r="P23" s="40"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="48"/>
+      <c r="P23" s="48"/>
       <c r="Q23" s="12"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="11"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="40"/>
-      <c r="O24" s="40"/>
-      <c r="P24" s="40"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="48"/>
+      <c r="O24" s="48"/>
+      <c r="P24" s="48"/>
       <c r="Q24" s="12"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="11"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
-      <c r="M25" s="40"/>
-      <c r="N25" s="40"/>
-      <c r="O25" s="40"/>
-      <c r="P25" s="40"/>
+      <c r="K25" s="48"/>
+      <c r="L25" s="48"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="48"/>
+      <c r="O25" s="48"/>
+      <c r="P25" s="48"/>
       <c r="Q25" s="12"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
-      <c r="M26" s="40"/>
-      <c r="N26" s="40"/>
-      <c r="O26" s="40"/>
-      <c r="P26" s="40"/>
+      <c r="K26" s="48"/>
+      <c r="L26" s="48"/>
+      <c r="M26" s="48"/>
+      <c r="N26" s="48"/>
+      <c r="O26" s="48"/>
+      <c r="P26" s="48"/>
       <c r="Q26" s="12"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="11"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="40"/>
-      <c r="L27" s="40"/>
-      <c r="M27" s="40"/>
-      <c r="N27" s="40"/>
-      <c r="O27" s="40"/>
-      <c r="P27" s="40"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="48"/>
+      <c r="M27" s="48"/>
+      <c r="N27" s="48"/>
+      <c r="O27" s="48"/>
+      <c r="P27" s="48"/>
       <c r="Q27" s="12"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="11"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="40"/>
-      <c r="L28" s="40"/>
-      <c r="M28" s="40"/>
-      <c r="N28" s="40"/>
-      <c r="O28" s="40"/>
-      <c r="P28" s="40"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="48"/>
+      <c r="O28" s="48"/>
+      <c r="P28" s="48"/>
       <c r="Q28" s="12"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="11"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="40"/>
-      <c r="N29" s="40"/>
-      <c r="O29" s="40"/>
-      <c r="P29" s="40"/>
+      <c r="K29" s="48"/>
+      <c r="L29" s="48"/>
+      <c r="M29" s="48"/>
+      <c r="N29" s="48"/>
+      <c r="O29" s="48"/>
+      <c r="P29" s="48"/>
       <c r="Q29" s="12"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="11"/>
       <c r="C30" s="5"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="40"/>
-      <c r="L30" s="40"/>
-      <c r="M30" s="40"/>
-      <c r="N30" s="40"/>
-      <c r="O30" s="40"/>
-      <c r="P30" s="40"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="48"/>
+      <c r="O30" s="48"/>
+      <c r="P30" s="48"/>
       <c r="Q30" s="12"/>
     </row>
-    <row r="31" spans="2:17" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:17" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="11"/>
       <c r="Q31" s="12"/>
     </row>
-    <row r="32" spans="2:17" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:17" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="11"/>
-      <c r="C32" s="55" t="s">
+      <c r="C32" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="55"/>
-      <c r="E32" s="55"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="55"/>
-      <c r="J32" s="55"/>
-      <c r="K32" s="55"/>
-      <c r="L32" s="55"/>
-      <c r="M32" s="55"/>
-      <c r="N32" s="55"/>
-      <c r="O32" s="55"/>
-      <c r="P32" s="55"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="63"/>
+      <c r="O32" s="63"/>
+      <c r="P32" s="63"/>
       <c r="Q32" s="12"/>
     </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" s="11"/>
       <c r="Q33" s="12"/>
     </row>
-    <row r="34" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="11"/>
-      <c r="C34" s="51" t="s">
+      <c r="C34" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
-      <c r="H34" s="51"/>
-      <c r="I34" s="51"/>
-      <c r="J34" s="51"/>
-      <c r="K34" s="51"/>
-      <c r="L34" s="51"/>
-      <c r="M34" s="51"/>
-      <c r="N34" s="51"/>
-      <c r="O34" s="51"/>
-      <c r="P34" s="51"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="59"/>
+      <c r="J34" s="59"/>
+      <c r="K34" s="59"/>
+      <c r="L34" s="59"/>
+      <c r="M34" s="59"/>
+      <c r="N34" s="59"/>
+      <c r="O34" s="59"/>
+      <c r="P34" s="59"/>
       <c r="Q34" s="12"/>
     </row>
-    <row r="35" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="11"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="39"/>
-      <c r="M35" s="39"/>
-      <c r="N35" s="39"/>
-      <c r="O35" s="39"/>
-      <c r="P35" s="39"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="47"/>
+      <c r="L35" s="47"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="47"/>
+      <c r="O35" s="47"/>
+      <c r="P35" s="47"/>
       <c r="Q35" s="12"/>
     </row>
-    <row r="36" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="11"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="59"/>
-      <c r="H36" s="59"/>
-      <c r="I36" s="59"/>
-      <c r="J36" s="59"/>
-      <c r="K36" s="59"/>
-      <c r="L36" s="59"/>
-      <c r="M36" s="59"/>
-      <c r="N36" s="59"/>
-      <c r="O36" s="59"/>
-      <c r="P36" s="59"/>
+      <c r="C36" s="67"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="67"/>
+      <c r="I36" s="67"/>
+      <c r="J36" s="67"/>
+      <c r="K36" s="67"/>
+      <c r="L36" s="67"/>
+      <c r="M36" s="67"/>
+      <c r="N36" s="67"/>
+      <c r="O36" s="67"/>
+      <c r="P36" s="67"/>
       <c r="Q36" s="12"/>
     </row>
-    <row r="37" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="11"/>
-      <c r="C37" s="59"/>
-      <c r="D37" s="59"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="59"/>
-      <c r="H37" s="59"/>
-      <c r="I37" s="59"/>
-      <c r="J37" s="59"/>
-      <c r="K37" s="59"/>
-      <c r="L37" s="59"/>
-      <c r="M37" s="59"/>
-      <c r="N37" s="59"/>
-      <c r="O37" s="59"/>
-      <c r="P37" s="59"/>
+      <c r="C37" s="67"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="67"/>
+      <c r="G37" s="67"/>
+      <c r="H37" s="67"/>
+      <c r="I37" s="67"/>
+      <c r="J37" s="67"/>
+      <c r="K37" s="67"/>
+      <c r="L37" s="67"/>
+      <c r="M37" s="67"/>
+      <c r="N37" s="67"/>
+      <c r="O37" s="67"/>
+      <c r="P37" s="67"/>
       <c r="Q37" s="12"/>
       <c r="T37">
         <f>1546-1378</f>
         <v>168</v>
       </c>
     </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B38" s="11"/>
       <c r="C38" s="17" t="s">
         <v>5</v>
       </c>
       <c r="Q38" s="12"/>
     </row>
-    <row r="39" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="11"/>
       <c r="Q39" s="12"/>
     </row>
-    <row r="40" spans="2:20" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:20" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="11"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="40"/>
-      <c r="G40" s="40"/>
-      <c r="H40" s="40"/>
-      <c r="I40" s="40"/>
-      <c r="J40" s="65"/>
-      <c r="K40" s="70"/>
-      <c r="L40" s="71"/>
-      <c r="M40" s="70"/>
-      <c r="N40" s="71"/>
-      <c r="O40" s="70"/>
-      <c r="P40" s="71"/>
+      <c r="C40" s="48"/>
+      <c r="D40" s="48"/>
+      <c r="E40" s="48"/>
+      <c r="F40" s="48"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="48"/>
+      <c r="I40" s="48"/>
+      <c r="J40" s="73"/>
+      <c r="K40" s="78"/>
+      <c r="L40" s="79"/>
+      <c r="M40" s="78"/>
+      <c r="N40" s="79"/>
+      <c r="O40" s="78"/>
+      <c r="P40" s="79"/>
       <c r="Q40" s="12"/>
     </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B41" s="11"/>
-      <c r="C41" s="58" t="s">
+      <c r="C41" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="D41" s="58"/>
-      <c r="E41" s="58" t="s">
+      <c r="D41" s="66"/>
+      <c r="E41" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="F41" s="58"/>
-      <c r="G41" s="58" t="s">
+      <c r="F41" s="66"/>
+      <c r="G41" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="H41" s="58"/>
-      <c r="I41" s="58"/>
-      <c r="J41" s="66"/>
-      <c r="K41" s="61" t="s">
+      <c r="H41" s="66"/>
+      <c r="I41" s="66"/>
+      <c r="J41" s="74"/>
+      <c r="K41" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="L41" s="62"/>
-      <c r="M41" s="61" t="s">
+      <c r="L41" s="70"/>
+      <c r="M41" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="N41" s="62"/>
-      <c r="O41" s="61" t="s">
+      <c r="N41" s="70"/>
+      <c r="O41" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="P41" s="62"/>
+      <c r="P41" s="70"/>
       <c r="Q41" s="12"/>
     </row>
-    <row r="42" spans="2:20" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:20" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="11"/>
-      <c r="C42" s="58"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="58"/>
-      <c r="F42" s="58"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="58"/>
-      <c r="I42" s="58"/>
-      <c r="J42" s="63" t="s">
+      <c r="C42" s="66"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="66"/>
+      <c r="F42" s="66"/>
+      <c r="G42" s="66"/>
+      <c r="H42" s="66"/>
+      <c r="I42" s="66"/>
+      <c r="J42" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="K42" s="67"/>
-      <c r="L42" s="68"/>
-      <c r="M42" s="68"/>
-      <c r="N42" s="68"/>
-      <c r="O42" s="68"/>
-      <c r="P42" s="69"/>
+      <c r="K42" s="75"/>
+      <c r="L42" s="76"/>
+      <c r="M42" s="76"/>
+      <c r="N42" s="76"/>
+      <c r="O42" s="76"/>
+      <c r="P42" s="77"/>
       <c r="Q42" s="12"/>
     </row>
-    <row r="43" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="11"/>
-      <c r="C43" s="58" t="s">
+      <c r="C43" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58" t="s">
+      <c r="D43" s="66"/>
+      <c r="E43" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="F43" s="58"/>
-      <c r="G43" s="58" t="s">
+      <c r="F43" s="66"/>
+      <c r="G43" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="64"/>
-      <c r="K43" s="67" t="s">
+      <c r="H43" s="66"/>
+      <c r="I43" s="66"/>
+      <c r="J43" s="72"/>
+      <c r="K43" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="L43" s="68"/>
-      <c r="M43" s="68"/>
-      <c r="N43" s="68"/>
-      <c r="O43" s="68"/>
-      <c r="P43" s="69"/>
+      <c r="L43" s="76"/>
+      <c r="M43" s="76"/>
+      <c r="N43" s="76"/>
+      <c r="O43" s="76"/>
+      <c r="P43" s="77"/>
       <c r="Q43" s="12"/>
     </row>
-    <row r="44" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="11"/>
       <c r="C44" s="21"/>
       <c r="D44" s="21"/>
@@ -3155,38 +2993,38 @@
       <c r="I44" s="21"/>
       <c r="J44" s="22"/>
       <c r="K44" s="22"/>
-      <c r="L44" s="60"/>
-      <c r="M44" s="60"/>
-      <c r="N44" s="60"/>
-      <c r="O44" s="60"/>
-      <c r="P44" s="60"/>
+      <c r="L44" s="68"/>
+      <c r="M44" s="68"/>
+      <c r="N44" s="68"/>
+      <c r="O44" s="68"/>
+      <c r="P44" s="68"/>
       <c r="Q44" s="12"/>
     </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B45" s="11"/>
       <c r="Q45" s="12"/>
     </row>
-    <row r="46" spans="2:20" ht="93.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:20" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="11"/>
-      <c r="C46" s="57" t="s">
+      <c r="C46" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="D46" s="57"/>
-      <c r="E46" s="57"/>
-      <c r="F46" s="57"/>
-      <c r="G46" s="57"/>
-      <c r="H46" s="57"/>
-      <c r="I46" s="57"/>
-      <c r="J46" s="57"/>
-      <c r="K46" s="57"/>
-      <c r="L46" s="57"/>
-      <c r="M46" s="57"/>
-      <c r="N46" s="57"/>
-      <c r="O46" s="57"/>
-      <c r="P46" s="57"/>
+      <c r="D46" s="65"/>
+      <c r="E46" s="65"/>
+      <c r="F46" s="65"/>
+      <c r="G46" s="65"/>
+      <c r="H46" s="65"/>
+      <c r="I46" s="65"/>
+      <c r="J46" s="65"/>
+      <c r="K46" s="65"/>
+      <c r="L46" s="65"/>
+      <c r="M46" s="65"/>
+      <c r="N46" s="65"/>
+      <c r="O46" s="65"/>
+      <c r="P46" s="65"/>
       <c r="Q46" s="12"/>
     </row>
-    <row r="47" spans="2:20" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:20" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="18"/>
       <c r="C47" s="19"/>
       <c r="D47" s="19"/>
@@ -3204,7 +3042,7 @@
       <c r="P47" s="19"/>
       <c r="Q47" s="20"/>
     </row>
-    <row r="48" spans="2:20" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="77">
     <mergeCell ref="D21:E21"/>
@@ -3310,146 +3148,146 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF3B689-9F06-47C4-AF24-1D135A215254}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF3B689-9F06-47C4-AF24-1D135A215254}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+      <selection activeCell="J21" sqref="J21:K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="17.25" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="31" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" style="28" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="28" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" style="28" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" style="28" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" style="31" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="28" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="28" customWidth="1"/>
+    <col min="5" max="5" width="5" style="28" customWidth="1"/>
     <col min="6" max="6" width="15" style="28" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" style="28" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" style="28" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" style="28" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="28" customWidth="1"/>
     <col min="9" max="9" width="9" style="28" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" style="28" customWidth="1"/>
-    <col min="11" max="11" width="32.6640625" style="28" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" style="28" customWidth="1"/>
-    <col min="13" max="13" width="47.21875" style="28" customWidth="1"/>
-    <col min="14" max="14" width="14.5546875" style="28" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" style="28" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" style="28" customWidth="1"/>
+    <col min="11" max="11" width="32.7109375" style="28" customWidth="1"/>
+    <col min="12" max="12" width="31.140625" style="28" customWidth="1"/>
+    <col min="13" max="13" width="47.28515625" style="28" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" style="28" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="28" customWidth="1"/>
     <col min="16" max="16" width="4" style="28" customWidth="1"/>
-    <col min="17" max="17" width="16.5546875" style="28" customWidth="1"/>
-    <col min="18" max="18" width="13.33203125" style="28" customWidth="1"/>
-    <col min="19" max="19" width="4.6640625" style="28" customWidth="1"/>
-    <col min="20" max="20" width="9.5546875" style="28" customWidth="1"/>
-    <col min="21" max="21" width="3.6640625" style="28" customWidth="1"/>
-    <col min="22" max="22" width="11.33203125" style="28" customWidth="1"/>
-    <col min="23" max="23" width="4.6640625" style="31" customWidth="1"/>
-    <col min="24" max="16384" width="11.44140625" style="28" hidden="1"/>
+    <col min="17" max="17" width="16.5703125" style="28" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" style="28" customWidth="1"/>
+    <col min="19" max="19" width="4.7109375" style="28" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" style="28" customWidth="1"/>
+    <col min="21" max="21" width="3.7109375" style="28" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" style="28" customWidth="1"/>
+    <col min="23" max="23" width="4.7109375" style="31" customWidth="1"/>
+    <col min="24" max="16384" width="11.42578125" style="28" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" s="31" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="115"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="97" t="s">
+    <row r="1" spans="2:22" s="31" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="123"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="109" t="s">
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="107"/>
+      <c r="M2" s="117" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="110"/>
-      <c r="O2" s="110"/>
-      <c r="P2" s="110"/>
-      <c r="Q2" s="110"/>
-      <c r="R2" s="110"/>
-      <c r="S2" s="110"/>
-      <c r="T2" s="110"/>
-      <c r="U2" s="110"/>
-      <c r="V2" s="111"/>
-    </row>
-    <row r="3" spans="2:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="118"/>
-      <c r="C3" s="119"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
-      <c r="L3" s="102"/>
-      <c r="M3" s="109" t="s">
+      <c r="N2" s="118"/>
+      <c r="O2" s="118"/>
+      <c r="P2" s="118"/>
+      <c r="Q2" s="118"/>
+      <c r="R2" s="118"/>
+      <c r="S2" s="118"/>
+      <c r="T2" s="118"/>
+      <c r="U2" s="118"/>
+      <c r="V2" s="119"/>
+    </row>
+    <row r="3" spans="2:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="126"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
+      <c r="K3" s="109"/>
+      <c r="L3" s="110"/>
+      <c r="M3" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="110"/>
-      <c r="O3" s="110"/>
-      <c r="P3" s="110"/>
-      <c r="Q3" s="110"/>
-      <c r="R3" s="110"/>
-      <c r="S3" s="110"/>
-      <c r="T3" s="110"/>
-      <c r="U3" s="110"/>
-      <c r="V3" s="111"/>
-    </row>
-    <row r="4" spans="2:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="103" t="s">
+      <c r="N3" s="118"/>
+      <c r="O3" s="118"/>
+      <c r="P3" s="118"/>
+      <c r="Q3" s="118"/>
+      <c r="R3" s="118"/>
+      <c r="S3" s="118"/>
+      <c r="T3" s="118"/>
+      <c r="U3" s="118"/>
+      <c r="V3" s="119"/>
+    </row>
+    <row r="4" spans="2:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="104"/>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
-      <c r="F4" s="104"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="105"/>
-      <c r="M4" s="112" t="s">
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="112"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="113"/>
+      <c r="M4" s="120" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="113"/>
-      <c r="O4" s="113"/>
-      <c r="P4" s="113"/>
-      <c r="Q4" s="113"/>
-      <c r="R4" s="113"/>
-      <c r="S4" s="113"/>
-      <c r="T4" s="113"/>
-      <c r="U4" s="113"/>
-      <c r="V4" s="114"/>
-    </row>
-    <row r="5" spans="2:22" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="106"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
-      <c r="J5" s="107"/>
-      <c r="K5" s="107"/>
-      <c r="L5" s="108"/>
-      <c r="M5" s="130" t="s">
+      <c r="N4" s="121"/>
+      <c r="O4" s="121"/>
+      <c r="P4" s="121"/>
+      <c r="Q4" s="121"/>
+      <c r="R4" s="121"/>
+      <c r="S4" s="121"/>
+      <c r="T4" s="121"/>
+      <c r="U4" s="121"/>
+      <c r="V4" s="122"/>
+    </row>
+    <row r="5" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="114"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
+      <c r="H5" s="115"/>
+      <c r="I5" s="115"/>
+      <c r="J5" s="115"/>
+      <c r="K5" s="115"/>
+      <c r="L5" s="116"/>
+      <c r="M5" s="138" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="131"/>
-      <c r="O5" s="129"/>
+      <c r="N5" s="139"/>
+      <c r="O5" s="137"/>
       <c r="P5" s="27"/>
-      <c r="Q5" s="128" t="s">
+      <c r="Q5" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="R5" s="129"/>
+      <c r="R5" s="137"/>
       <c r="S5" s="32"/>
       <c r="T5" s="27" t="s">
         <v>13</v>
@@ -3457,694 +3295,694 @@
       <c r="U5" s="26"/>
       <c r="V5" s="29"/>
     </row>
-    <row r="6" spans="2:22" s="31" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="90" t="s">
+    <row r="6" spans="2:22" s="31" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="92"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="132"/>
-      <c r="F7" s="132"/>
-      <c r="G7" s="132"/>
-      <c r="H7" s="132"/>
-      <c r="I7" s="132"/>
-      <c r="J7" s="132"/>
-      <c r="K7" s="132"/>
-      <c r="L7" s="92" t="s">
+      <c r="C7" s="102"/>
+      <c r="D7" s="102"/>
+      <c r="E7" s="140"/>
+      <c r="F7" s="140"/>
+      <c r="G7" s="140"/>
+      <c r="H7" s="140"/>
+      <c r="I7" s="140"/>
+      <c r="J7" s="140"/>
+      <c r="K7" s="140"/>
+      <c r="L7" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="M7" s="92"/>
-      <c r="N7" s="92"/>
-      <c r="O7" s="73"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
-      <c r="R7" s="74"/>
-      <c r="S7" s="74"/>
-      <c r="T7" s="74"/>
-      <c r="U7" s="74"/>
-      <c r="V7" s="75"/>
-    </row>
-    <row r="8" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="91" t="s">
+      <c r="M7" s="102"/>
+      <c r="N7" s="102"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="82"/>
+      <c r="Q7" s="82"/>
+      <c r="R7" s="82"/>
+      <c r="S7" s="82"/>
+      <c r="T7" s="82"/>
+      <c r="U7" s="82"/>
+      <c r="V7" s="83"/>
+    </row>
+    <row r="8" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="93" t="s">
+      <c r="C8" s="101"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="101" t="s">
         <v>28</v>
       </c>
-      <c r="M8" s="93"/>
-      <c r="N8" s="93"/>
-      <c r="O8" s="76"/>
-      <c r="P8" s="77"/>
-      <c r="Q8" s="77"/>
-      <c r="R8" s="77"/>
-      <c r="S8" s="77"/>
-      <c r="T8" s="77"/>
-      <c r="U8" s="77"/>
-      <c r="V8" s="78"/>
-    </row>
-    <row r="9" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="91" t="s">
+      <c r="M8" s="101"/>
+      <c r="N8" s="101"/>
+      <c r="O8" s="84"/>
+      <c r="P8" s="85"/>
+      <c r="Q8" s="85"/>
+      <c r="R8" s="85"/>
+      <c r="S8" s="85"/>
+      <c r="T8" s="85"/>
+      <c r="U8" s="85"/>
+      <c r="V8" s="86"/>
+    </row>
+    <row r="9" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="93"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="93" t="s">
+      <c r="C9" s="101"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="90"/>
+      <c r="G9" s="90"/>
+      <c r="H9" s="101" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="93"/>
-      <c r="J9" s="93"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
-      <c r="M9" s="94"/>
-      <c r="N9" s="93" t="s">
+      <c r="I9" s="101"/>
+      <c r="J9" s="101"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="O9" s="93"/>
-      <c r="P9" s="93"/>
-      <c r="Q9" s="93"/>
-      <c r="R9" s="93"/>
-      <c r="S9" s="93"/>
-      <c r="T9" s="94" t="str">
+      <c r="O9" s="101"/>
+      <c r="P9" s="101"/>
+      <c r="Q9" s="101"/>
+      <c r="R9" s="101"/>
+      <c r="S9" s="101"/>
+      <c r="T9" s="90" t="str">
         <f>IFERROR(VLOOKUP(K9,Hoja3!B5:C7,2,FALSE)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U9" s="94"/>
-      <c r="V9" s="123"/>
-    </row>
-    <row r="10" spans="2:22" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="124" t="s">
+      <c r="U9" s="90"/>
+      <c r="V9" s="131"/>
+    </row>
+    <row r="10" spans="2:22" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="132" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="125"/>
-      <c r="D10" s="125"/>
-      <c r="E10" s="126"/>
-      <c r="F10" s="126"/>
-      <c r="G10" s="126"/>
-      <c r="H10" s="126"/>
-      <c r="I10" s="126"/>
-      <c r="J10" s="126"/>
-      <c r="K10" s="126"/>
-      <c r="L10" s="126"/>
-      <c r="M10" s="126"/>
-      <c r="N10" s="125" t="s">
+      <c r="C10" s="133"/>
+      <c r="D10" s="133"/>
+      <c r="E10" s="134"/>
+      <c r="F10" s="134"/>
+      <c r="G10" s="134"/>
+      <c r="H10" s="134"/>
+      <c r="I10" s="134"/>
+      <c r="J10" s="134"/>
+      <c r="K10" s="134"/>
+      <c r="L10" s="134"/>
+      <c r="M10" s="134"/>
+      <c r="N10" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="O10" s="125"/>
-      <c r="P10" s="125"/>
-      <c r="Q10" s="125"/>
-      <c r="R10" s="125"/>
-      <c r="S10" s="125"/>
-      <c r="T10" s="126"/>
-      <c r="U10" s="126"/>
-      <c r="V10" s="127"/>
-    </row>
-    <row r="11" spans="2:22" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="2:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="90" t="s">
+      <c r="O10" s="133"/>
+      <c r="P10" s="133"/>
+      <c r="Q10" s="133"/>
+      <c r="R10" s="133"/>
+      <c r="S10" s="133"/>
+      <c r="T10" s="134"/>
+      <c r="U10" s="134"/>
+      <c r="V10" s="135"/>
+    </row>
+    <row r="11" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="2:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="99" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="92" t="s">
+      <c r="C12" s="102" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="92"/>
-      <c r="E12" s="92"/>
-      <c r="F12" s="92" t="s">
+      <c r="D12" s="102"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="92" t="s">
+      <c r="G12" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="92" t="s">
+      <c r="H12" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="92"/>
-      <c r="J12" s="92" t="s">
+      <c r="I12" s="102"/>
+      <c r="J12" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="K12" s="92"/>
-      <c r="L12" s="92"/>
-      <c r="M12" s="92" t="s">
+      <c r="K12" s="102"/>
+      <c r="L12" s="102"/>
+      <c r="M12" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="N12" s="92" t="s">
+      <c r="N12" s="102" t="s">
         <v>61</v>
       </c>
-      <c r="O12" s="92"/>
-      <c r="P12" s="92"/>
-      <c r="Q12" s="92"/>
-      <c r="R12" s="92" t="s">
+      <c r="O12" s="102"/>
+      <c r="P12" s="102"/>
+      <c r="Q12" s="102"/>
+      <c r="R12" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="S12" s="92"/>
-      <c r="T12" s="92"/>
-      <c r="U12" s="92"/>
-      <c r="V12" s="95"/>
-    </row>
-    <row r="13" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="91"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="93"/>
-      <c r="G13" s="93"/>
-      <c r="H13" s="93"/>
-      <c r="I13" s="93"/>
-      <c r="J13" s="93" t="s">
+      <c r="S12" s="102"/>
+      <c r="T12" s="102"/>
+      <c r="U12" s="102"/>
+      <c r="V12" s="103"/>
+    </row>
+    <row r="13" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="100"/>
+      <c r="C13" s="101"/>
+      <c r="D13" s="101"/>
+      <c r="E13" s="101"/>
+      <c r="F13" s="101"/>
+      <c r="G13" s="101"/>
+      <c r="H13" s="101"/>
+      <c r="I13" s="101"/>
+      <c r="J13" s="101" t="s">
         <v>69</v>
       </c>
-      <c r="K13" s="93"/>
+      <c r="K13" s="101"/>
       <c r="L13" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="M13" s="93"/>
-      <c r="N13" s="93"/>
-      <c r="O13" s="93"/>
-      <c r="P13" s="93"/>
-      <c r="Q13" s="93"/>
-      <c r="R13" s="93"/>
-      <c r="S13" s="93"/>
-      <c r="T13" s="93"/>
-      <c r="U13" s="93"/>
-      <c r="V13" s="96"/>
-    </row>
-    <row r="14" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="133"/>
-      <c r="C14" s="79"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
+      <c r="M13" s="101"/>
+      <c r="N13" s="101"/>
+      <c r="O13" s="101"/>
+      <c r="P13" s="101"/>
+      <c r="Q13" s="101"/>
+      <c r="R13" s="101"/>
+      <c r="S13" s="101"/>
+      <c r="T13" s="101"/>
+      <c r="U13" s="101"/>
+      <c r="V13" s="104"/>
+    </row>
+    <row r="14" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="39"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="91"/>
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
-      <c r="H14" s="79"/>
-      <c r="I14" s="79"/>
-      <c r="J14" s="79"/>
-      <c r="K14" s="79"/>
-      <c r="L14" s="134"/>
+      <c r="H14" s="91"/>
+      <c r="I14" s="91"/>
+      <c r="J14" s="91"/>
+      <c r="K14" s="91"/>
+      <c r="L14" s="40"/>
       <c r="M14" s="33"/>
-      <c r="N14" s="79"/>
-      <c r="O14" s="79"/>
-      <c r="P14" s="79"/>
-      <c r="Q14" s="79"/>
-      <c r="R14" s="79"/>
-      <c r="S14" s="79"/>
-      <c r="T14" s="79"/>
-      <c r="U14" s="79"/>
-      <c r="V14" s="80"/>
-    </row>
-    <row r="15" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="133"/>
-      <c r="C15" s="79"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
+      <c r="N14" s="91"/>
+      <c r="O14" s="91"/>
+      <c r="P14" s="91"/>
+      <c r="Q14" s="91"/>
+      <c r="R14" s="91"/>
+      <c r="S14" s="91"/>
+      <c r="T14" s="91"/>
+      <c r="U14" s="91"/>
+      <c r="V14" s="92"/>
+    </row>
+    <row r="15" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="39"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
       <c r="F15" s="37"/>
       <c r="G15" s="37"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="79"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="79"/>
-      <c r="L15" s="134"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="91"/>
+      <c r="J15" s="91"/>
+      <c r="K15" s="91"/>
+      <c r="L15" s="40"/>
       <c r="M15" s="33"/>
-      <c r="N15" s="79"/>
-      <c r="O15" s="79"/>
-      <c r="P15" s="79"/>
-      <c r="Q15" s="79"/>
-      <c r="R15" s="79"/>
-      <c r="S15" s="79"/>
-      <c r="T15" s="79"/>
-      <c r="U15" s="79"/>
-      <c r="V15" s="80"/>
-    </row>
-    <row r="16" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="133"/>
-      <c r="C16" s="79"/>
-      <c r="D16" s="79"/>
-      <c r="E16" s="79"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="91"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
+      <c r="R15" s="91"/>
+      <c r="S15" s="91"/>
+      <c r="T15" s="91"/>
+      <c r="U15" s="91"/>
+      <c r="V15" s="92"/>
+    </row>
+    <row r="16" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="39"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="91"/>
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="79"/>
-      <c r="J16" s="79"/>
-      <c r="K16" s="79"/>
-      <c r="L16" s="134"/>
+      <c r="H16" s="91"/>
+      <c r="I16" s="91"/>
+      <c r="J16" s="91"/>
+      <c r="K16" s="91"/>
+      <c r="L16" s="40"/>
       <c r="M16" s="33"/>
-      <c r="N16" s="79"/>
-      <c r="O16" s="79"/>
-      <c r="P16" s="79"/>
-      <c r="Q16" s="79"/>
-      <c r="R16" s="79"/>
-      <c r="S16" s="79"/>
-      <c r="T16" s="79"/>
-      <c r="U16" s="79"/>
-      <c r="V16" s="80"/>
-    </row>
-    <row r="17" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="133"/>
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="79"/>
+      <c r="N16" s="91"/>
+      <c r="O16" s="91"/>
+      <c r="P16" s="91"/>
+      <c r="Q16" s="91"/>
+      <c r="R16" s="91"/>
+      <c r="S16" s="91"/>
+      <c r="T16" s="91"/>
+      <c r="U16" s="91"/>
+      <c r="V16" s="92"/>
+    </row>
+    <row r="17" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="39"/>
+      <c r="C17" s="91"/>
+      <c r="D17" s="91"/>
+      <c r="E17" s="91"/>
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
-      <c r="H17" s="79"/>
-      <c r="I17" s="79"/>
-      <c r="J17" s="79"/>
-      <c r="K17" s="79"/>
-      <c r="L17" s="134"/>
+      <c r="H17" s="91"/>
+      <c r="I17" s="91"/>
+      <c r="J17" s="91"/>
+      <c r="K17" s="91"/>
+      <c r="L17" s="40"/>
       <c r="M17" s="33"/>
-      <c r="N17" s="79"/>
-      <c r="O17" s="79"/>
-      <c r="P17" s="79"/>
-      <c r="Q17" s="79"/>
-      <c r="R17" s="79"/>
-      <c r="S17" s="79"/>
-      <c r="T17" s="79"/>
-      <c r="U17" s="79"/>
-      <c r="V17" s="80"/>
-    </row>
-    <row r="18" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="133"/>
-      <c r="C18" s="94"/>
-      <c r="D18" s="94"/>
-      <c r="E18" s="94"/>
+      <c r="N17" s="91"/>
+      <c r="O17" s="91"/>
+      <c r="P17" s="91"/>
+      <c r="Q17" s="91"/>
+      <c r="R17" s="91"/>
+      <c r="S17" s="91"/>
+      <c r="T17" s="91"/>
+      <c r="U17" s="91"/>
+      <c r="V17" s="92"/>
+    </row>
+    <row r="18" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="39"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="90"/>
+      <c r="E18" s="90"/>
       <c r="F18" s="37"/>
       <c r="G18" s="37"/>
-      <c r="H18" s="79"/>
-      <c r="I18" s="79"/>
-      <c r="J18" s="79"/>
-      <c r="K18" s="79"/>
-      <c r="L18" s="134"/>
+      <c r="H18" s="91"/>
+      <c r="I18" s="91"/>
+      <c r="J18" s="91"/>
+      <c r="K18" s="91"/>
+      <c r="L18" s="40"/>
       <c r="M18" s="33"/>
-      <c r="N18" s="79"/>
-      <c r="O18" s="79"/>
-      <c r="P18" s="79"/>
-      <c r="Q18" s="79"/>
-      <c r="R18" s="79"/>
-      <c r="S18" s="79"/>
-      <c r="T18" s="79"/>
-      <c r="U18" s="79"/>
-      <c r="V18" s="80"/>
-    </row>
-    <row r="19" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="133"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
+      <c r="N18" s="91"/>
+      <c r="O18" s="91"/>
+      <c r="P18" s="91"/>
+      <c r="Q18" s="91"/>
+      <c r="R18" s="91"/>
+      <c r="S18" s="91"/>
+      <c r="T18" s="91"/>
+      <c r="U18" s="91"/>
+      <c r="V18" s="92"/>
+    </row>
+    <row r="19" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="39"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="91"/>
+      <c r="E19" s="91"/>
       <c r="F19" s="37"/>
       <c r="G19" s="37"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="79"/>
-      <c r="J19" s="79"/>
-      <c r="K19" s="79"/>
-      <c r="L19" s="134"/>
+      <c r="H19" s="91"/>
+      <c r="I19" s="91"/>
+      <c r="J19" s="91"/>
+      <c r="K19" s="91"/>
+      <c r="L19" s="40"/>
       <c r="M19" s="33"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="79"/>
-      <c r="P19" s="79"/>
-      <c r="Q19" s="79"/>
-      <c r="R19" s="79"/>
-      <c r="S19" s="79"/>
-      <c r="T19" s="79"/>
-      <c r="U19" s="79"/>
-      <c r="V19" s="80"/>
-    </row>
-    <row r="20" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="133"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="79"/>
-      <c r="E20" s="79"/>
+      <c r="N19" s="91"/>
+      <c r="O19" s="91"/>
+      <c r="P19" s="91"/>
+      <c r="Q19" s="91"/>
+      <c r="R19" s="91"/>
+      <c r="S19" s="91"/>
+      <c r="T19" s="91"/>
+      <c r="U19" s="91"/>
+      <c r="V19" s="92"/>
+    </row>
+    <row r="20" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="39"/>
+      <c r="C20" s="91"/>
+      <c r="D20" s="91"/>
+      <c r="E20" s="91"/>
       <c r="F20" s="37"/>
       <c r="G20" s="37"/>
-      <c r="H20" s="79"/>
-      <c r="I20" s="79"/>
-      <c r="J20" s="79"/>
-      <c r="K20" s="79"/>
-      <c r="L20" s="134"/>
+      <c r="H20" s="91"/>
+      <c r="I20" s="91"/>
+      <c r="J20" s="91"/>
+      <c r="K20" s="91"/>
+      <c r="L20" s="40"/>
       <c r="M20" s="33"/>
-      <c r="N20" s="79"/>
-      <c r="O20" s="79"/>
-      <c r="P20" s="79"/>
-      <c r="Q20" s="79"/>
-      <c r="R20" s="79"/>
-      <c r="S20" s="79"/>
-      <c r="T20" s="79"/>
-      <c r="U20" s="79"/>
-      <c r="V20" s="80"/>
-    </row>
-    <row r="21" spans="2:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="135"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
+      <c r="N20" s="91"/>
+      <c r="O20" s="91"/>
+      <c r="P20" s="91"/>
+      <c r="Q20" s="91"/>
+      <c r="R20" s="91"/>
+      <c r="S20" s="91"/>
+      <c r="T20" s="91"/>
+      <c r="U20" s="91"/>
+      <c r="V20" s="92"/>
+    </row>
+    <row r="21" spans="2:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="41"/>
+      <c r="C21" s="98"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="98"/>
       <c r="F21" s="38"/>
       <c r="G21" s="38"/>
-      <c r="H21" s="81"/>
-      <c r="I21" s="81"/>
-      <c r="J21" s="81"/>
-      <c r="K21" s="81"/>
-      <c r="L21" s="136"/>
+      <c r="H21" s="98"/>
+      <c r="I21" s="98"/>
+      <c r="J21" s="98"/>
+      <c r="K21" s="98"/>
+      <c r="L21" s="40"/>
       <c r="M21" s="34"/>
-      <c r="N21" s="81"/>
-      <c r="O21" s="81"/>
-      <c r="P21" s="81"/>
-      <c r="Q21" s="81"/>
-      <c r="R21" s="81"/>
-      <c r="S21" s="81"/>
-      <c r="T21" s="81"/>
-      <c r="U21" s="81"/>
-      <c r="V21" s="82"/>
-    </row>
-    <row r="22" spans="2:23" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="2:23" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="87" t="s">
+      <c r="N21" s="98"/>
+      <c r="O21" s="98"/>
+      <c r="P21" s="98"/>
+      <c r="Q21" s="98"/>
+      <c r="R21" s="98"/>
+      <c r="S21" s="98"/>
+      <c r="T21" s="98"/>
+      <c r="U21" s="98"/>
+      <c r="V21" s="141"/>
+    </row>
+    <row r="22" spans="2:23" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="2:23" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="142" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="88"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
-      <c r="G23" s="88"/>
-      <c r="H23" s="88"/>
-      <c r="I23" s="88"/>
-      <c r="J23" s="88"/>
-      <c r="K23" s="88"/>
-      <c r="L23" s="88"/>
-      <c r="M23" s="88"/>
-      <c r="N23" s="88"/>
-      <c r="O23" s="88"/>
-      <c r="P23" s="88"/>
-      <c r="Q23" s="88"/>
-      <c r="R23" s="88"/>
-      <c r="S23" s="88"/>
-      <c r="T23" s="88"/>
-      <c r="U23" s="88"/>
-      <c r="V23" s="89"/>
-    </row>
-    <row r="24" spans="2:23" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="167"/>
-      <c r="C24" s="167"/>
-      <c r="D24" s="167"/>
-      <c r="E24" s="167"/>
-      <c r="F24" s="167"/>
-      <c r="G24" s="167"/>
-      <c r="H24" s="167"/>
-      <c r="I24" s="167"/>
-      <c r="J24" s="167"/>
-      <c r="K24" s="167"/>
-      <c r="L24" s="167"/>
-      <c r="M24" s="167"/>
-      <c r="N24" s="167"/>
-      <c r="O24" s="167"/>
-      <c r="P24" s="167"/>
-      <c r="Q24" s="167"/>
-      <c r="R24" s="167"/>
-      <c r="S24" s="167"/>
-      <c r="T24" s="167"/>
-      <c r="U24" s="167"/>
-      <c r="V24" s="167"/>
+      <c r="C23" s="143"/>
+      <c r="D23" s="143"/>
+      <c r="E23" s="143"/>
+      <c r="F23" s="143"/>
+      <c r="G23" s="143"/>
+      <c r="H23" s="143"/>
+      <c r="I23" s="143"/>
+      <c r="J23" s="143"/>
+      <c r="K23" s="143"/>
+      <c r="L23" s="143"/>
+      <c r="M23" s="143"/>
+      <c r="N23" s="143"/>
+      <c r="O23" s="143"/>
+      <c r="P23" s="143"/>
+      <c r="Q23" s="143"/>
+      <c r="R23" s="143"/>
+      <c r="S23" s="143"/>
+      <c r="T23" s="143"/>
+      <c r="U23" s="143"/>
+      <c r="V23" s="144"/>
+    </row>
+    <row r="24" spans="2:23" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="155"/>
+      <c r="C24" s="155"/>
+      <c r="D24" s="155"/>
+      <c r="E24" s="155"/>
+      <c r="F24" s="155"/>
+      <c r="G24" s="155"/>
+      <c r="H24" s="155"/>
+      <c r="I24" s="155"/>
+      <c r="J24" s="155"/>
+      <c r="K24" s="155"/>
+      <c r="L24" s="155"/>
+      <c r="M24" s="155"/>
+      <c r="N24" s="155"/>
+      <c r="O24" s="155"/>
+      <c r="P24" s="155"/>
+      <c r="Q24" s="155"/>
+      <c r="R24" s="155"/>
+      <c r="S24" s="155"/>
+      <c r="T24" s="155"/>
+      <c r="U24" s="155"/>
+      <c r="V24" s="155"/>
       <c r="W24" s="28"/>
     </row>
-    <row r="25" spans="2:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="B25" s="31"/>
       <c r="W25" s="28"/>
     </row>
-    <row r="26" spans="2:23" ht="0.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:23" ht="0.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="31"/>
       <c r="W26" s="28"/>
     </row>
-    <row r="27" spans="2:23" ht="27.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:23" ht="27.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="31"/>
       <c r="W27" s="28"/>
     </row>
-    <row r="28" spans="2:23" ht="27.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:23" ht="27.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="31"/>
       <c r="W28" s="28"/>
     </row>
-    <row r="29" spans="2:23" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="137" t="s">
+    <row r="29" spans="2:23" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="138"/>
-      <c r="D29" s="138"/>
-      <c r="E29" s="138"/>
-      <c r="F29" s="138"/>
-      <c r="G29" s="138"/>
-      <c r="H29" s="138"/>
-      <c r="I29" s="138"/>
-      <c r="J29" s="138"/>
-      <c r="K29" s="138"/>
-      <c r="L29" s="138"/>
-      <c r="M29" s="138"/>
-      <c r="N29" s="138"/>
-      <c r="O29" s="138"/>
-      <c r="P29" s="138"/>
-      <c r="Q29" s="138"/>
-      <c r="R29" s="138"/>
-      <c r="S29" s="138"/>
-      <c r="T29" s="138"/>
-      <c r="U29" s="138"/>
-      <c r="V29" s="139"/>
-    </row>
-    <row r="30" spans="2:23" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="137" t="s">
+      <c r="C29" s="94"/>
+      <c r="D29" s="94"/>
+      <c r="E29" s="94"/>
+      <c r="F29" s="94"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="94"/>
+      <c r="I29" s="94"/>
+      <c r="J29" s="94"/>
+      <c r="K29" s="94"/>
+      <c r="L29" s="94"/>
+      <c r="M29" s="94"/>
+      <c r="N29" s="94"/>
+      <c r="O29" s="94"/>
+      <c r="P29" s="94"/>
+      <c r="Q29" s="94"/>
+      <c r="R29" s="94"/>
+      <c r="S29" s="94"/>
+      <c r="T29" s="94"/>
+      <c r="U29" s="94"/>
+      <c r="V29" s="95"/>
+    </row>
+    <row r="30" spans="2:23" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="93" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="138"/>
-      <c r="D30" s="138"/>
-      <c r="E30" s="138"/>
-      <c r="F30" s="138"/>
-      <c r="G30" s="139"/>
-      <c r="H30" s="137" t="s">
+      <c r="C30" s="94"/>
+      <c r="D30" s="94"/>
+      <c r="E30" s="94"/>
+      <c r="F30" s="94"/>
+      <c r="G30" s="95"/>
+      <c r="H30" s="93" t="s">
         <v>71</v>
       </c>
-      <c r="I30" s="138"/>
-      <c r="J30" s="138"/>
-      <c r="K30" s="139"/>
-      <c r="L30" s="137" t="s">
+      <c r="I30" s="94"/>
+      <c r="J30" s="94"/>
+      <c r="K30" s="95"/>
+      <c r="L30" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="M30" s="139"/>
-      <c r="N30" s="168" t="s">
+      <c r="M30" s="95"/>
+      <c r="N30" s="156" t="s">
         <v>73</v>
       </c>
-      <c r="O30" s="169"/>
-      <c r="P30" s="169"/>
-      <c r="Q30" s="170"/>
-      <c r="R30" s="137" t="s">
+      <c r="O30" s="157"/>
+      <c r="P30" s="157"/>
+      <c r="Q30" s="158"/>
+      <c r="R30" s="93" t="s">
         <v>74</v>
       </c>
-      <c r="S30" s="138"/>
-      <c r="T30" s="138"/>
-      <c r="U30" s="138"/>
-      <c r="V30" s="139"/>
-    </row>
-    <row r="31" spans="2:23" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="171" t="s">
+      <c r="S30" s="94"/>
+      <c r="T30" s="94"/>
+      <c r="U30" s="94"/>
+      <c r="V30" s="95"/>
+    </row>
+    <row r="31" spans="2:23" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="172"/>
-      <c r="D31" s="85"/>
-      <c r="E31" s="173"/>
-      <c r="F31" s="173"/>
-      <c r="G31" s="174"/>
-      <c r="H31" s="140" t="s">
+      <c r="C31" s="97"/>
+      <c r="D31" s="87"/>
+      <c r="E31" s="88"/>
+      <c r="F31" s="88"/>
+      <c r="G31" s="89"/>
+      <c r="H31" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="I31" s="175"/>
-      <c r="J31" s="176"/>
-      <c r="K31" s="177"/>
-      <c r="L31" s="140" t="s">
+      <c r="I31" s="159"/>
+      <c r="J31" s="160"/>
+      <c r="K31" s="161"/>
+      <c r="L31" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="M31" s="141"/>
+      <c r="M31" s="43"/>
       <c r="N31" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="O31" s="142"/>
-      <c r="P31" s="143"/>
-      <c r="Q31" s="178"/>
-      <c r="R31" s="140" t="s">
+      <c r="O31" s="162"/>
+      <c r="P31" s="163"/>
+      <c r="Q31" s="164"/>
+      <c r="R31" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="S31" s="85"/>
-      <c r="T31" s="173"/>
-      <c r="U31" s="173"/>
-      <c r="V31" s="174"/>
-    </row>
-    <row r="32" spans="2:23" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="83" t="s">
+      <c r="S31" s="87"/>
+      <c r="T31" s="88"/>
+      <c r="U31" s="88"/>
+      <c r="V31" s="89"/>
+    </row>
+    <row r="32" spans="2:23" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="150" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="84"/>
-      <c r="D32" s="81"/>
-      <c r="E32" s="81"/>
-      <c r="F32" s="81"/>
-      <c r="G32" s="144"/>
+      <c r="C32" s="165"/>
+      <c r="D32" s="98"/>
+      <c r="E32" s="98"/>
+      <c r="F32" s="98"/>
+      <c r="G32" s="166"/>
       <c r="H32" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="I32" s="145"/>
-      <c r="J32" s="146"/>
-      <c r="K32" s="147"/>
+      <c r="I32" s="167"/>
+      <c r="J32" s="168"/>
+      <c r="K32" s="169"/>
       <c r="L32" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="M32" s="148"/>
+      <c r="M32" s="44"/>
       <c r="N32" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="O32" s="145"/>
-      <c r="P32" s="146"/>
-      <c r="Q32" s="147"/>
+      <c r="O32" s="167"/>
+      <c r="P32" s="168"/>
+      <c r="Q32" s="169"/>
       <c r="R32" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="S32" s="144"/>
-      <c r="T32" s="149"/>
-      <c r="U32" s="149"/>
-      <c r="V32" s="150"/>
-    </row>
-    <row r="33" spans="2:22" ht="11.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="2:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="151" t="s">
+      <c r="S32" s="166"/>
+      <c r="T32" s="170"/>
+      <c r="U32" s="170"/>
+      <c r="V32" s="171"/>
+    </row>
+    <row r="33" spans="2:22" ht="11.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="2:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="172" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="152"/>
-      <c r="D34" s="152"/>
-      <c r="E34" s="152"/>
-      <c r="F34" s="152"/>
-      <c r="G34" s="152"/>
-      <c r="H34" s="152"/>
-      <c r="I34" s="152"/>
-      <c r="J34" s="152"/>
-      <c r="K34" s="153"/>
-      <c r="L34" s="151" t="s">
+      <c r="C34" s="173"/>
+      <c r="D34" s="173"/>
+      <c r="E34" s="173"/>
+      <c r="F34" s="173"/>
+      <c r="G34" s="173"/>
+      <c r="H34" s="173"/>
+      <c r="I34" s="173"/>
+      <c r="J34" s="173"/>
+      <c r="K34" s="174"/>
+      <c r="L34" s="172" t="s">
         <v>76</v>
       </c>
-      <c r="M34" s="152"/>
-      <c r="N34" s="152"/>
-      <c r="O34" s="152"/>
-      <c r="P34" s="152"/>
-      <c r="Q34" s="152"/>
-      <c r="R34" s="152"/>
-      <c r="S34" s="152"/>
-      <c r="T34" s="152"/>
-      <c r="U34" s="152"/>
-      <c r="V34" s="153"/>
-    </row>
-    <row r="35" spans="2:22" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="154"/>
-      <c r="C35" s="155"/>
-      <c r="D35" s="155"/>
-      <c r="E35" s="155"/>
-      <c r="F35" s="155"/>
-      <c r="G35" s="155"/>
-      <c r="H35" s="155"/>
-      <c r="I35" s="155"/>
-      <c r="J35" s="155"/>
-      <c r="K35" s="156"/>
-      <c r="L35" s="154"/>
-      <c r="M35" s="155"/>
-      <c r="N35" s="155"/>
-      <c r="O35" s="155"/>
-      <c r="P35" s="155"/>
-      <c r="Q35" s="155"/>
-      <c r="R35" s="155"/>
-      <c r="S35" s="155"/>
-      <c r="T35" s="155"/>
-      <c r="U35" s="155"/>
-      <c r="V35" s="156"/>
-    </row>
-    <row r="36" spans="2:22" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="86" t="s">
+      <c r="M34" s="173"/>
+      <c r="N34" s="173"/>
+      <c r="O34" s="173"/>
+      <c r="P34" s="173"/>
+      <c r="Q34" s="173"/>
+      <c r="R34" s="173"/>
+      <c r="S34" s="173"/>
+      <c r="T34" s="173"/>
+      <c r="U34" s="173"/>
+      <c r="V34" s="174"/>
+    </row>
+    <row r="35" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="175"/>
+      <c r="C35" s="176"/>
+      <c r="D35" s="176"/>
+      <c r="E35" s="176"/>
+      <c r="F35" s="176"/>
+      <c r="G35" s="176"/>
+      <c r="H35" s="176"/>
+      <c r="I35" s="176"/>
+      <c r="J35" s="176"/>
+      <c r="K35" s="177"/>
+      <c r="L35" s="175"/>
+      <c r="M35" s="176"/>
+      <c r="N35" s="176"/>
+      <c r="O35" s="176"/>
+      <c r="P35" s="176"/>
+      <c r="Q35" s="176"/>
+      <c r="R35" s="176"/>
+      <c r="S35" s="176"/>
+      <c r="T35" s="176"/>
+      <c r="U35" s="176"/>
+      <c r="V35" s="177"/>
+    </row>
+    <row r="36" spans="2:22" ht="31.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="145" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="157"/>
-      <c r="D36" s="158"/>
-      <c r="E36" s="159"/>
-      <c r="F36" s="159"/>
-      <c r="G36" s="159"/>
-      <c r="H36" s="159"/>
-      <c r="I36" s="159"/>
-      <c r="J36" s="159"/>
-      <c r="K36" s="160"/>
-      <c r="L36" s="161" t="s">
+      <c r="C36" s="146"/>
+      <c r="D36" s="147"/>
+      <c r="E36" s="148"/>
+      <c r="F36" s="148"/>
+      <c r="G36" s="148"/>
+      <c r="H36" s="148"/>
+      <c r="I36" s="148"/>
+      <c r="J36" s="148"/>
+      <c r="K36" s="149"/>
+      <c r="L36" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="M36" s="159"/>
-      <c r="N36" s="159"/>
-      <c r="O36" s="159"/>
-      <c r="P36" s="159"/>
-      <c r="Q36" s="159"/>
-      <c r="R36" s="159"/>
-      <c r="S36" s="159"/>
-      <c r="T36" s="159"/>
-      <c r="U36" s="159"/>
-      <c r="V36" s="160"/>
-    </row>
-    <row r="37" spans="2:22" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="83" t="s">
+      <c r="M36" s="148"/>
+      <c r="N36" s="148"/>
+      <c r="O36" s="148"/>
+      <c r="P36" s="148"/>
+      <c r="Q36" s="148"/>
+      <c r="R36" s="148"/>
+      <c r="S36" s="148"/>
+      <c r="T36" s="148"/>
+      <c r="U36" s="148"/>
+      <c r="V36" s="149"/>
+    </row>
+    <row r="37" spans="2:22" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="150" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="162"/>
-      <c r="D37" s="163"/>
-      <c r="E37" s="119"/>
-      <c r="F37" s="119"/>
-      <c r="G37" s="119"/>
-      <c r="H37" s="119"/>
-      <c r="I37" s="119"/>
-      <c r="J37" s="119"/>
-      <c r="K37" s="164"/>
-      <c r="L37" s="165" t="s">
+      <c r="C37" s="151"/>
+      <c r="D37" s="152"/>
+      <c r="E37" s="127"/>
+      <c r="F37" s="127"/>
+      <c r="G37" s="127"/>
+      <c r="H37" s="127"/>
+      <c r="I37" s="127"/>
+      <c r="J37" s="127"/>
+      <c r="K37" s="153"/>
+      <c r="L37" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="M37" s="166"/>
-      <c r="N37" s="166"/>
-      <c r="O37" s="166"/>
-      <c r="P37" s="166"/>
-      <c r="Q37" s="166"/>
-      <c r="R37" s="166"/>
-      <c r="S37" s="166"/>
-      <c r="T37" s="166"/>
-      <c r="U37" s="166"/>
-      <c r="V37" s="120"/>
-    </row>
-    <row r="38" spans="2:22" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="121" t="s">
+      <c r="M37" s="154"/>
+      <c r="N37" s="154"/>
+      <c r="O37" s="154"/>
+      <c r="P37" s="154"/>
+      <c r="Q37" s="154"/>
+      <c r="R37" s="154"/>
+      <c r="S37" s="154"/>
+      <c r="T37" s="154"/>
+      <c r="U37" s="154"/>
+      <c r="V37" s="128"/>
+    </row>
+    <row r="38" spans="2:22" ht="109.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="129" t="s">
         <v>66</v>
       </c>
-      <c r="C38" s="122"/>
-      <c r="D38" s="122"/>
-      <c r="E38" s="122"/>
-      <c r="F38" s="122"/>
-      <c r="G38" s="122"/>
-      <c r="H38" s="122"/>
-      <c r="I38" s="122"/>
-      <c r="J38" s="122"/>
-      <c r="K38" s="122"/>
-      <c r="L38" s="122"/>
-      <c r="M38" s="122"/>
-      <c r="N38" s="122"/>
-      <c r="O38" s="122"/>
-      <c r="P38" s="122"/>
-      <c r="Q38" s="122"/>
-      <c r="R38" s="122"/>
-      <c r="S38" s="122"/>
-      <c r="T38" s="122"/>
-      <c r="U38" s="122"/>
-      <c r="V38" s="122"/>
-    </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.25"/>
+      <c r="C38" s="130"/>
+      <c r="D38" s="130"/>
+      <c r="E38" s="130"/>
+      <c r="F38" s="130"/>
+      <c r="G38" s="130"/>
+      <c r="H38" s="130"/>
+      <c r="I38" s="130"/>
+      <c r="J38" s="130"/>
+      <c r="K38" s="130"/>
+      <c r="L38" s="130"/>
+      <c r="M38" s="130"/>
+      <c r="N38" s="130"/>
+      <c r="O38" s="130"/>
+      <c r="P38" s="130"/>
+      <c r="Q38" s="130"/>
+      <c r="R38" s="130"/>
+      <c r="S38" s="130"/>
+      <c r="T38" s="130"/>
+      <c r="U38" s="130"/>
+      <c r="V38" s="130"/>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="103">
     <mergeCell ref="B36:C36"/>
@@ -4180,6 +4018,7 @@
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="N20:Q20"/>
     <mergeCell ref="R20:V20"/>
+    <mergeCell ref="B23:V23"/>
     <mergeCell ref="E2:L3"/>
     <mergeCell ref="B4:L5"/>
     <mergeCell ref="M2:V2"/>
@@ -4225,17 +4064,9 @@
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="N15:Q15"/>
     <mergeCell ref="R15:V15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="R16:V16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="R17:V17"/>
-    <mergeCell ref="B23:V23"/>
+    <mergeCell ref="O7:V7"/>
+    <mergeCell ref="O8:V8"/>
+    <mergeCell ref="D31:G31"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="J18:K18"/>
@@ -4247,65 +4078,21 @@
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="J21:K21"/>
-    <mergeCell ref="O7:V7"/>
-    <mergeCell ref="O8:V8"/>
-    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="R16:V16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="R17:V17"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="56" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2050" r:id="rId4" name="Check Box 2">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>19</xdr:col>
-                    <xdr:colOff>350520</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>45720</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>20</xdr:col>
-                    <xdr:colOff>106680</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>441960</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2051" r:id="rId5" name="Check Box 3">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>20</xdr:col>
-                    <xdr:colOff>236220</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>38100</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>21</xdr:col>
-                    <xdr:colOff>411480</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>441960</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-  </mc:AlternateContent>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -4335,14 +4122,14 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>34</v>
       </c>
@@ -4353,7 +4140,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>35</v>
       </c>
@@ -4364,7 +4151,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>36</v>
       </c>
@@ -4375,7 +4162,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>55</v>
       </c>
@@ -4386,27 +4173,27 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D8" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D9" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D10" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D11" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
CAMBIOS IMPORTANTES FINALIZACION CAMUNDA DEMO
</commit_message>
<xml_diff>
--- a/templates/plantilla.xlsx
+++ b/templates/plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\Requisiciones\camunda_back\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E2C755-D1F4-4CC7-AE96-E4C300BCB4FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFAD2A3-F8B4-4D98-A490-52C2D96042BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" firstSheet="1" activeTab="1" xr2:uid="{6CC2AB2B-0F37-47AE-B363-6A70476DA6B2}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="78">
   <si>
     <t>DESCRIPCIÓN (DETALLADA)</t>
   </si>
@@ -1202,7 +1202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1306,8 +1306,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1411,7 +1411,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1492,6 +1504,9 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1549,12 +1564,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1588,15 +1597,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1648,18 +1648,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1678,23 +1666,26 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3187,8 +3178,8 @@
   </sheetPr>
   <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="71" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33:V33"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="17.25" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -3196,7 +3187,7 @@
     <col min="1" max="1" width="4.140625" style="31" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" style="28" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="28" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" style="28" customWidth="1"/>
     <col min="5" max="5" width="5" style="28" customWidth="1"/>
     <col min="6" max="6" width="15" style="28" customWidth="1"/>
     <col min="7" max="7" width="21.85546875" style="28" customWidth="1"/>
@@ -3221,106 +3212,106 @@
   <sheetData>
     <row r="1" spans="2:22" s="31" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="120"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="103" t="s">
+      <c r="B2" s="125"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="104"/>
-      <c r="K2" s="104"/>
-      <c r="L2" s="105"/>
-      <c r="M2" s="114" t="s">
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
+      <c r="K2" s="108"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="115"/>
-      <c r="O2" s="115"/>
-      <c r="P2" s="115"/>
-      <c r="Q2" s="115"/>
-      <c r="R2" s="115"/>
-      <c r="S2" s="115"/>
-      <c r="T2" s="115"/>
-      <c r="U2" s="115"/>
-      <c r="V2" s="116"/>
+      <c r="N2" s="120"/>
+      <c r="O2" s="120"/>
+      <c r="P2" s="120"/>
+      <c r="Q2" s="120"/>
+      <c r="R2" s="120"/>
+      <c r="S2" s="120"/>
+      <c r="T2" s="120"/>
+      <c r="U2" s="120"/>
+      <c r="V2" s="121"/>
     </row>
     <row r="3" spans="2:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="123"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="125"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="114" t="s">
+      <c r="B3" s="128"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="110"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="112"/>
+      <c r="M3" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="115"/>
-      <c r="O3" s="115"/>
-      <c r="P3" s="115"/>
-      <c r="Q3" s="115"/>
-      <c r="R3" s="115"/>
-      <c r="S3" s="115"/>
-      <c r="T3" s="115"/>
-      <c r="U3" s="115"/>
-      <c r="V3" s="116"/>
+      <c r="N3" s="120"/>
+      <c r="O3" s="120"/>
+      <c r="P3" s="120"/>
+      <c r="Q3" s="120"/>
+      <c r="R3" s="120"/>
+      <c r="S3" s="120"/>
+      <c r="T3" s="120"/>
+      <c r="U3" s="120"/>
+      <c r="V3" s="121"/>
     </row>
     <row r="4" spans="2:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="108" t="s">
+      <c r="B4" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="109"/>
-      <c r="D4" s="109"/>
-      <c r="E4" s="109"/>
-      <c r="F4" s="109"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="109"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="109"/>
-      <c r="K4" s="109"/>
-      <c r="L4" s="110"/>
-      <c r="M4" s="117" t="s">
+      <c r="C4" s="114"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="114"/>
+      <c r="G4" s="114"/>
+      <c r="H4" s="114"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="114"/>
+      <c r="K4" s="114"/>
+      <c r="L4" s="115"/>
+      <c r="M4" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="118"/>
-      <c r="O4" s="118"/>
-      <c r="P4" s="118"/>
-      <c r="Q4" s="118"/>
-      <c r="R4" s="118"/>
-      <c r="S4" s="118"/>
-      <c r="T4" s="118"/>
-      <c r="U4" s="118"/>
-      <c r="V4" s="119"/>
+      <c r="N4" s="123"/>
+      <c r="O4" s="123"/>
+      <c r="P4" s="123"/>
+      <c r="Q4" s="123"/>
+      <c r="R4" s="123"/>
+      <c r="S4" s="123"/>
+      <c r="T4" s="123"/>
+      <c r="U4" s="123"/>
+      <c r="V4" s="124"/>
     </row>
     <row r="5" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="111"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
-      <c r="H5" s="112"/>
-      <c r="I5" s="112"/>
-      <c r="J5" s="112"/>
-      <c r="K5" s="112"/>
-      <c r="L5" s="113"/>
-      <c r="M5" s="135" t="s">
+      <c r="B5" s="116"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117"/>
+      <c r="E5" s="117"/>
+      <c r="F5" s="117"/>
+      <c r="G5" s="117"/>
+      <c r="H5" s="117"/>
+      <c r="I5" s="117"/>
+      <c r="J5" s="117"/>
+      <c r="K5" s="117"/>
+      <c r="L5" s="118"/>
+      <c r="M5" s="138" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="136"/>
-      <c r="O5" s="134"/>
+      <c r="N5" s="139"/>
+      <c r="O5" s="137"/>
       <c r="P5" s="27"/>
-      <c r="Q5" s="133" t="s">
+      <c r="Q5" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="R5" s="134"/>
+      <c r="R5" s="137"/>
       <c r="S5" s="32"/>
       <c r="T5" s="27" t="s">
         <v>13</v>
@@ -3330,396 +3321,396 @@
     </row>
     <row r="6" spans="2:22" s="31" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="137"/>
-      <c r="F7" s="137"/>
-      <c r="G7" s="137"/>
-      <c r="H7" s="137"/>
-      <c r="I7" s="137"/>
-      <c r="J7" s="137"/>
-      <c r="K7" s="137"/>
-      <c r="L7" s="100" t="s">
+      <c r="C7" s="104"/>
+      <c r="D7" s="104"/>
+      <c r="E7" s="140"/>
+      <c r="F7" s="140"/>
+      <c r="G7" s="140"/>
+      <c r="H7" s="140"/>
+      <c r="I7" s="140"/>
+      <c r="J7" s="140"/>
+      <c r="K7" s="140"/>
+      <c r="L7" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="M7" s="100"/>
-      <c r="N7" s="100"/>
-      <c r="O7" s="81"/>
-      <c r="P7" s="82"/>
-      <c r="Q7" s="82"/>
-      <c r="R7" s="82"/>
-      <c r="S7" s="82"/>
-      <c r="T7" s="82"/>
-      <c r="U7" s="82"/>
-      <c r="V7" s="83"/>
+      <c r="M7" s="104"/>
+      <c r="N7" s="104"/>
+      <c r="O7" s="85"/>
+      <c r="P7" s="86"/>
+      <c r="Q7" s="86"/>
+      <c r="R7" s="86"/>
+      <c r="S7" s="86"/>
+      <c r="T7" s="86"/>
+      <c r="U7" s="86"/>
+      <c r="V7" s="87"/>
     </row>
     <row r="8" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="99"/>
-      <c r="D8" s="99"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="88"/>
-      <c r="I8" s="88"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="88"/>
-      <c r="L8" s="99" t="s">
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="92"/>
+      <c r="F8" s="92"/>
+      <c r="G8" s="92"/>
+      <c r="H8" s="92"/>
+      <c r="I8" s="92"/>
+      <c r="J8" s="92"/>
+      <c r="K8" s="92"/>
+      <c r="L8" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="M8" s="99"/>
-      <c r="N8" s="99"/>
-      <c r="O8" s="84"/>
-      <c r="P8" s="85"/>
-      <c r="Q8" s="85"/>
-      <c r="R8" s="85"/>
-      <c r="S8" s="85"/>
-      <c r="T8" s="85"/>
-      <c r="U8" s="85"/>
-      <c r="V8" s="86"/>
+      <c r="M8" s="103"/>
+      <c r="N8" s="103"/>
+      <c r="O8" s="88"/>
+      <c r="P8" s="89"/>
+      <c r="Q8" s="89"/>
+      <c r="R8" s="89"/>
+      <c r="S8" s="89"/>
+      <c r="T8" s="89"/>
+      <c r="U8" s="89"/>
+      <c r="V8" s="90"/>
     </row>
     <row r="9" spans="2:22" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="98" t="s">
+      <c r="B9" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="88"/>
-      <c r="H9" s="99" t="s">
+      <c r="C9" s="103"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="99"/>
-      <c r="J9" s="99"/>
-      <c r="K9" s="88"/>
-      <c r="L9" s="88"/>
-      <c r="M9" s="88"/>
-      <c r="N9" s="99" t="s">
+      <c r="I9" s="103"/>
+      <c r="J9" s="103"/>
+      <c r="K9" s="92"/>
+      <c r="L9" s="92"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="O9" s="99"/>
-      <c r="P9" s="99"/>
-      <c r="Q9" s="99"/>
-      <c r="R9" s="99"/>
-      <c r="S9" s="99"/>
-      <c r="T9" s="88" t="str">
+      <c r="O9" s="103"/>
+      <c r="P9" s="103"/>
+      <c r="Q9" s="103"/>
+      <c r="R9" s="103"/>
+      <c r="S9" s="103"/>
+      <c r="T9" s="92" t="str">
         <f>IFERROR(VLOOKUP(K9,Hoja3!B5:C7,2,FALSE)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U9" s="88"/>
-      <c r="V9" s="128"/>
+      <c r="U9" s="92"/>
+      <c r="V9" s="131"/>
     </row>
     <row r="10" spans="2:22" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="129" t="s">
+      <c r="B10" s="132" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="130"/>
-      <c r="D10" s="130"/>
-      <c r="E10" s="131"/>
-      <c r="F10" s="131"/>
-      <c r="G10" s="131"/>
-      <c r="H10" s="131"/>
-      <c r="I10" s="131"/>
-      <c r="J10" s="131"/>
-      <c r="K10" s="131"/>
-      <c r="L10" s="131"/>
-      <c r="M10" s="131"/>
-      <c r="N10" s="130" t="s">
+      <c r="C10" s="133"/>
+      <c r="D10" s="133"/>
+      <c r="E10" s="134"/>
+      <c r="F10" s="134"/>
+      <c r="G10" s="134"/>
+      <c r="H10" s="134"/>
+      <c r="I10" s="134"/>
+      <c r="J10" s="134"/>
+      <c r="K10" s="134"/>
+      <c r="L10" s="134"/>
+      <c r="M10" s="134"/>
+      <c r="N10" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="O10" s="130"/>
-      <c r="P10" s="130"/>
-      <c r="Q10" s="130"/>
-      <c r="R10" s="130"/>
-      <c r="S10" s="130"/>
-      <c r="T10" s="131"/>
-      <c r="U10" s="131"/>
-      <c r="V10" s="132"/>
+      <c r="O10" s="133"/>
+      <c r="P10" s="133"/>
+      <c r="Q10" s="133"/>
+      <c r="R10" s="133"/>
+      <c r="S10" s="133"/>
+      <c r="T10" s="134"/>
+      <c r="U10" s="134"/>
+      <c r="V10" s="135"/>
     </row>
     <row r="11" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="2:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="97" t="s">
+    <row r="12" spans="2:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="101" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="100" t="s">
+      <c r="C12" s="104" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="100"/>
-      <c r="E12" s="100"/>
-      <c r="F12" s="100" t="s">
+      <c r="D12" s="104"/>
+      <c r="E12" s="104"/>
+      <c r="F12" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="100" t="s">
+      <c r="G12" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="100" t="s">
+      <c r="H12" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="100"/>
-      <c r="J12" s="100" t="s">
+      <c r="I12" s="104"/>
+      <c r="J12" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="K12" s="100"/>
-      <c r="L12" s="100"/>
-      <c r="M12" s="100" t="s">
+      <c r="K12" s="104"/>
+      <c r="L12" s="104"/>
+      <c r="M12" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="N12" s="100" t="s">
+      <c r="N12" s="104" t="s">
         <v>61</v>
       </c>
-      <c r="O12" s="100"/>
-      <c r="P12" s="100"/>
-      <c r="Q12" s="100"/>
-      <c r="R12" s="100" t="s">
+      <c r="O12" s="104"/>
+      <c r="P12" s="104"/>
+      <c r="Q12" s="104"/>
+      <c r="R12" s="104" t="s">
         <v>68</v>
       </c>
-      <c r="S12" s="100"/>
-      <c r="T12" s="100"/>
-      <c r="U12" s="100"/>
-      <c r="V12" s="101"/>
+      <c r="S12" s="104"/>
+      <c r="T12" s="104"/>
+      <c r="U12" s="104"/>
+      <c r="V12" s="105"/>
     </row>
     <row r="13" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="98"/>
-      <c r="C13" s="99"/>
-      <c r="D13" s="99"/>
-      <c r="E13" s="99"/>
-      <c r="F13" s="99"/>
-      <c r="G13" s="99"/>
-      <c r="H13" s="99"/>
-      <c r="I13" s="99"/>
-      <c r="J13" s="99" t="s">
+      <c r="B13" s="102"/>
+      <c r="C13" s="103"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="103"/>
+      <c r="F13" s="103"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="103"/>
+      <c r="I13" s="103"/>
+      <c r="J13" s="103" t="s">
         <v>69</v>
       </c>
-      <c r="K13" s="99"/>
+      <c r="K13" s="103"/>
       <c r="L13" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="M13" s="99"/>
-      <c r="N13" s="99"/>
-      <c r="O13" s="99"/>
-      <c r="P13" s="99"/>
-      <c r="Q13" s="99"/>
-      <c r="R13" s="99"/>
-      <c r="S13" s="99"/>
-      <c r="T13" s="99"/>
-      <c r="U13" s="99"/>
-      <c r="V13" s="102"/>
+      <c r="M13" s="103"/>
+      <c r="N13" s="103"/>
+      <c r="O13" s="103"/>
+      <c r="P13" s="103"/>
+      <c r="Q13" s="103"/>
+      <c r="R13" s="103"/>
+      <c r="S13" s="103"/>
+      <c r="T13" s="103"/>
+      <c r="U13" s="103"/>
+      <c r="V13" s="106"/>
     </row>
     <row r="14" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="37"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="93"/>
+      <c r="E14" s="93"/>
       <c r="F14" s="35"/>
       <c r="G14" s="35"/>
-      <c r="H14" s="89"/>
-      <c r="I14" s="89"/>
-      <c r="J14" s="89"/>
-      <c r="K14" s="89"/>
+      <c r="H14" s="93"/>
+      <c r="I14" s="93"/>
+      <c r="J14" s="93"/>
+      <c r="K14" s="93"/>
       <c r="L14" s="38"/>
       <c r="M14" s="33"/>
-      <c r="N14" s="89"/>
-      <c r="O14" s="89"/>
-      <c r="P14" s="89"/>
-      <c r="Q14" s="89"/>
-      <c r="R14" s="89"/>
-      <c r="S14" s="89"/>
-      <c r="T14" s="89"/>
-      <c r="U14" s="89"/>
-      <c r="V14" s="90"/>
+      <c r="N14" s="93"/>
+      <c r="O14" s="93"/>
+      <c r="P14" s="93"/>
+      <c r="Q14" s="93"/>
+      <c r="R14" s="93"/>
+      <c r="S14" s="93"/>
+      <c r="T14" s="93"/>
+      <c r="U14" s="93"/>
+      <c r="V14" s="94"/>
     </row>
     <row r="15" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="37"/>
-      <c r="C15" s="89"/>
-      <c r="D15" s="89"/>
-      <c r="E15" s="89"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="93"/>
+      <c r="E15" s="93"/>
       <c r="F15" s="35"/>
       <c r="G15" s="35"/>
-      <c r="H15" s="89"/>
-      <c r="I15" s="89"/>
-      <c r="J15" s="89"/>
-      <c r="K15" s="89"/>
+      <c r="H15" s="93"/>
+      <c r="I15" s="93"/>
+      <c r="J15" s="93"/>
+      <c r="K15" s="93"/>
       <c r="L15" s="38"/>
       <c r="M15" s="33"/>
-      <c r="N15" s="89"/>
-      <c r="O15" s="89"/>
-      <c r="P15" s="89"/>
-      <c r="Q15" s="89"/>
-      <c r="R15" s="89"/>
-      <c r="S15" s="89"/>
-      <c r="T15" s="89"/>
-      <c r="U15" s="89"/>
-      <c r="V15" s="90"/>
+      <c r="N15" s="93"/>
+      <c r="O15" s="93"/>
+      <c r="P15" s="93"/>
+      <c r="Q15" s="93"/>
+      <c r="R15" s="93"/>
+      <c r="S15" s="93"/>
+      <c r="T15" s="93"/>
+      <c r="U15" s="93"/>
+      <c r="V15" s="94"/>
     </row>
     <row r="16" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="37"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="89"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
       <c r="F16" s="35"/>
       <c r="G16" s="35"/>
-      <c r="H16" s="89"/>
-      <c r="I16" s="89"/>
-      <c r="J16" s="89"/>
-      <c r="K16" s="89"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="93"/>
+      <c r="J16" s="93"/>
+      <c r="K16" s="93"/>
       <c r="L16" s="38"/>
       <c r="M16" s="33"/>
-      <c r="N16" s="89"/>
-      <c r="O16" s="89"/>
-      <c r="P16" s="89"/>
-      <c r="Q16" s="89"/>
-      <c r="R16" s="89"/>
-      <c r="S16" s="89"/>
-      <c r="T16" s="89"/>
-      <c r="U16" s="89"/>
-      <c r="V16" s="90"/>
+      <c r="N16" s="93"/>
+      <c r="O16" s="93"/>
+      <c r="P16" s="93"/>
+      <c r="Q16" s="93"/>
+      <c r="R16" s="93"/>
+      <c r="S16" s="93"/>
+      <c r="T16" s="93"/>
+      <c r="U16" s="93"/>
+      <c r="V16" s="94"/>
     </row>
     <row r="17" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="37"/>
-      <c r="C17" s="89"/>
-      <c r="D17" s="89"/>
-      <c r="E17" s="89"/>
+      <c r="C17" s="93"/>
+      <c r="D17" s="93"/>
+      <c r="E17" s="93"/>
       <c r="F17" s="35"/>
       <c r="G17" s="35"/>
-      <c r="H17" s="89"/>
-      <c r="I17" s="89"/>
-      <c r="J17" s="89"/>
-      <c r="K17" s="89"/>
+      <c r="H17" s="93"/>
+      <c r="I17" s="93"/>
+      <c r="J17" s="93"/>
+      <c r="K17" s="93"/>
       <c r="L17" s="38"/>
       <c r="M17" s="33"/>
-      <c r="N17" s="89"/>
-      <c r="O17" s="89"/>
-      <c r="P17" s="89"/>
-      <c r="Q17" s="89"/>
-      <c r="R17" s="89"/>
-      <c r="S17" s="89"/>
-      <c r="T17" s="89"/>
-      <c r="U17" s="89"/>
-      <c r="V17" s="90"/>
+      <c r="N17" s="93"/>
+      <c r="O17" s="93"/>
+      <c r="P17" s="93"/>
+      <c r="Q17" s="93"/>
+      <c r="R17" s="93"/>
+      <c r="S17" s="93"/>
+      <c r="T17" s="93"/>
+      <c r="U17" s="93"/>
+      <c r="V17" s="94"/>
     </row>
     <row r="18" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="37"/>
-      <c r="C18" s="88"/>
-      <c r="D18" s="88"/>
-      <c r="E18" s="88"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="92"/>
       <c r="F18" s="35"/>
       <c r="G18" s="35"/>
-      <c r="H18" s="89"/>
-      <c r="I18" s="89"/>
-      <c r="J18" s="89"/>
-      <c r="K18" s="89"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="93"/>
+      <c r="J18" s="93"/>
+      <c r="K18" s="93"/>
       <c r="L18" s="38"/>
       <c r="M18" s="33"/>
-      <c r="N18" s="89"/>
-      <c r="O18" s="89"/>
-      <c r="P18" s="89"/>
-      <c r="Q18" s="89"/>
-      <c r="R18" s="89"/>
-      <c r="S18" s="89"/>
-      <c r="T18" s="89"/>
-      <c r="U18" s="89"/>
-      <c r="V18" s="90"/>
+      <c r="N18" s="93"/>
+      <c r="O18" s="93"/>
+      <c r="P18" s="93"/>
+      <c r="Q18" s="93"/>
+      <c r="R18" s="93"/>
+      <c r="S18" s="93"/>
+      <c r="T18" s="93"/>
+      <c r="U18" s="93"/>
+      <c r="V18" s="94"/>
     </row>
     <row r="19" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="37"/>
-      <c r="C19" s="89"/>
-      <c r="D19" s="89"/>
-      <c r="E19" s="89"/>
+      <c r="C19" s="93"/>
+      <c r="D19" s="93"/>
+      <c r="E19" s="93"/>
       <c r="F19" s="35"/>
       <c r="G19" s="35"/>
-      <c r="H19" s="89"/>
-      <c r="I19" s="89"/>
-      <c r="J19" s="89"/>
-      <c r="K19" s="89"/>
+      <c r="H19" s="93"/>
+      <c r="I19" s="93"/>
+      <c r="J19" s="93"/>
+      <c r="K19" s="93"/>
       <c r="L19" s="38"/>
       <c r="M19" s="33"/>
-      <c r="N19" s="89"/>
-      <c r="O19" s="89"/>
-      <c r="P19" s="89"/>
-      <c r="Q19" s="89"/>
-      <c r="R19" s="89"/>
-      <c r="S19" s="89"/>
-      <c r="T19" s="89"/>
-      <c r="U19" s="89"/>
-      <c r="V19" s="90"/>
+      <c r="N19" s="93"/>
+      <c r="O19" s="93"/>
+      <c r="P19" s="93"/>
+      <c r="Q19" s="93"/>
+      <c r="R19" s="93"/>
+      <c r="S19" s="93"/>
+      <c r="T19" s="93"/>
+      <c r="U19" s="93"/>
+      <c r="V19" s="94"/>
     </row>
     <row r="20" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="37"/>
-      <c r="C20" s="89"/>
-      <c r="D20" s="89"/>
-      <c r="E20" s="89"/>
+      <c r="C20" s="93"/>
+      <c r="D20" s="93"/>
+      <c r="E20" s="93"/>
       <c r="F20" s="35"/>
       <c r="G20" s="35"/>
-      <c r="H20" s="89"/>
-      <c r="I20" s="89"/>
-      <c r="J20" s="89"/>
-      <c r="K20" s="89"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="93"/>
+      <c r="J20" s="93"/>
+      <c r="K20" s="93"/>
       <c r="L20" s="38"/>
       <c r="M20" s="33"/>
-      <c r="N20" s="89"/>
-      <c r="O20" s="89"/>
-      <c r="P20" s="89"/>
-      <c r="Q20" s="89"/>
-      <c r="R20" s="89"/>
-      <c r="S20" s="89"/>
-      <c r="T20" s="89"/>
-      <c r="U20" s="89"/>
-      <c r="V20" s="90"/>
+      <c r="N20" s="93"/>
+      <c r="O20" s="93"/>
+      <c r="P20" s="93"/>
+      <c r="Q20" s="93"/>
+      <c r="R20" s="93"/>
+      <c r="S20" s="93"/>
+      <c r="T20" s="93"/>
+      <c r="U20" s="93"/>
+      <c r="V20" s="94"/>
     </row>
     <row r="21" spans="2:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="39"/>
-      <c r="C21" s="96"/>
-      <c r="D21" s="96"/>
-      <c r="E21" s="96"/>
+      <c r="C21" s="100"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="100"/>
       <c r="F21" s="36"/>
       <c r="G21" s="36"/>
-      <c r="H21" s="96"/>
-      <c r="I21" s="96"/>
-      <c r="J21" s="96"/>
-      <c r="K21" s="96"/>
+      <c r="H21" s="100"/>
+      <c r="I21" s="100"/>
+      <c r="J21" s="100"/>
+      <c r="K21" s="100"/>
       <c r="L21" s="38"/>
       <c r="M21" s="34"/>
-      <c r="N21" s="96"/>
-      <c r="O21" s="96"/>
-      <c r="P21" s="96"/>
-      <c r="Q21" s="96"/>
-      <c r="R21" s="96"/>
-      <c r="S21" s="96"/>
-      <c r="T21" s="96"/>
-      <c r="U21" s="96"/>
-      <c r="V21" s="138"/>
+      <c r="N21" s="100"/>
+      <c r="O21" s="100"/>
+      <c r="P21" s="100"/>
+      <c r="Q21" s="100"/>
+      <c r="R21" s="100"/>
+      <c r="S21" s="100"/>
+      <c r="T21" s="100"/>
+      <c r="U21" s="100"/>
+      <c r="V21" s="141"/>
     </row>
     <row r="22" spans="2:23" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="23" spans="2:23" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="139" t="s">
+      <c r="B23" s="166" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="140"/>
-      <c r="D23" s="140"/>
-      <c r="E23" s="140"/>
-      <c r="F23" s="140"/>
-      <c r="G23" s="140"/>
-      <c r="H23" s="140"/>
-      <c r="I23" s="140"/>
-      <c r="J23" s="140"/>
-      <c r="K23" s="140"/>
-      <c r="L23" s="140"/>
-      <c r="M23" s="140"/>
-      <c r="N23" s="140"/>
-      <c r="O23" s="140"/>
-      <c r="P23" s="140"/>
-      <c r="Q23" s="140"/>
-      <c r="R23" s="140"/>
-      <c r="S23" s="140"/>
-      <c r="T23" s="140"/>
-      <c r="U23" s="140"/>
-      <c r="V23" s="141"/>
+      <c r="C23" s="167"/>
+      <c r="D23" s="167"/>
+      <c r="E23" s="167"/>
+      <c r="F23" s="167"/>
+      <c r="G23" s="167"/>
+      <c r="H23" s="167"/>
+      <c r="I23" s="167"/>
+      <c r="J23" s="167"/>
+      <c r="K23" s="167"/>
+      <c r="L23" s="167"/>
+      <c r="M23" s="167"/>
+      <c r="N23" s="167"/>
+      <c r="O23" s="167"/>
+      <c r="P23" s="167"/>
+      <c r="Q23" s="167"/>
+      <c r="R23" s="167"/>
+      <c r="S23" s="167"/>
+      <c r="T23" s="167"/>
+      <c r="U23" s="167"/>
+      <c r="V23" s="168"/>
     </row>
     <row r="24" spans="2:23" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="152"/>
@@ -3762,72 +3753,72 @@
       <c r="W28" s="28"/>
     </row>
     <row r="29" spans="2:23" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="91" t="s">
+      <c r="B29" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="92"/>
-      <c r="D29" s="92"/>
-      <c r="E29" s="92"/>
-      <c r="F29" s="92"/>
-      <c r="G29" s="92"/>
-      <c r="H29" s="92"/>
-      <c r="I29" s="92"/>
-      <c r="J29" s="92"/>
-      <c r="K29" s="92"/>
-      <c r="L29" s="92"/>
-      <c r="M29" s="92"/>
-      <c r="N29" s="92"/>
-      <c r="O29" s="92"/>
-      <c r="P29" s="92"/>
-      <c r="Q29" s="92"/>
-      <c r="R29" s="92"/>
-      <c r="S29" s="92"/>
-      <c r="T29" s="92"/>
-      <c r="U29" s="92"/>
-      <c r="V29" s="93"/>
+      <c r="C29" s="96"/>
+      <c r="D29" s="96"/>
+      <c r="E29" s="96"/>
+      <c r="F29" s="96"/>
+      <c r="G29" s="96"/>
+      <c r="H29" s="96"/>
+      <c r="I29" s="96"/>
+      <c r="J29" s="96"/>
+      <c r="K29" s="96"/>
+      <c r="L29" s="96"/>
+      <c r="M29" s="96"/>
+      <c r="N29" s="96"/>
+      <c r="O29" s="96"/>
+      <c r="P29" s="96"/>
+      <c r="Q29" s="96"/>
+      <c r="R29" s="96"/>
+      <c r="S29" s="96"/>
+      <c r="T29" s="96"/>
+      <c r="U29" s="96"/>
+      <c r="V29" s="97"/>
     </row>
     <row r="30" spans="2:23" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="91" t="s">
+      <c r="B30" s="95" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="92"/>
-      <c r="D30" s="92"/>
-      <c r="E30" s="92"/>
-      <c r="F30" s="92"/>
-      <c r="G30" s="93"/>
-      <c r="H30" s="91" t="s">
+      <c r="C30" s="96"/>
+      <c r="D30" s="96"/>
+      <c r="E30" s="96"/>
+      <c r="F30" s="96"/>
+      <c r="G30" s="97"/>
+      <c r="H30" s="95" t="s">
         <v>71</v>
       </c>
-      <c r="I30" s="92"/>
-      <c r="J30" s="92"/>
-      <c r="K30" s="93"/>
-      <c r="L30" s="91" t="s">
+      <c r="I30" s="96"/>
+      <c r="J30" s="96"/>
+      <c r="K30" s="97"/>
+      <c r="L30" s="95" t="s">
         <v>73</v>
       </c>
-      <c r="M30" s="93"/>
+      <c r="M30" s="97"/>
       <c r="N30" s="153" t="s">
         <v>72</v>
       </c>
       <c r="O30" s="154"/>
       <c r="P30" s="154"/>
       <c r="Q30" s="155"/>
-      <c r="R30" s="91" t="s">
+      <c r="R30" s="95" t="s">
         <v>74</v>
       </c>
-      <c r="S30" s="92"/>
-      <c r="T30" s="92"/>
-      <c r="U30" s="92"/>
-      <c r="V30" s="93"/>
+      <c r="S30" s="96"/>
+      <c r="T30" s="96"/>
+      <c r="U30" s="96"/>
+      <c r="V30" s="97"/>
     </row>
     <row r="31" spans="2:23" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="94" t="s">
+      <c r="B31" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="95"/>
-      <c r="D31" s="87"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="87"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="91"/>
+      <c r="E31" s="91"/>
+      <c r="F31" s="91"/>
+      <c r="G31" s="91"/>
       <c r="H31" s="42" t="s">
         <v>64</v>
       </c>
@@ -3847,215 +3838,183 @@
       <c r="R31" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="S31" s="87"/>
-      <c r="T31" s="87"/>
-      <c r="U31" s="87"/>
+      <c r="S31" s="91"/>
+      <c r="T31" s="91"/>
+      <c r="U31" s="91"/>
       <c r="V31" s="158"/>
     </row>
     <row r="32" spans="2:23" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="147" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="159"/>
-      <c r="D32" s="160"/>
-      <c r="E32" s="89"/>
-      <c r="F32" s="89"/>
-      <c r="G32" s="161"/>
+        <v>77</v>
+      </c>
+      <c r="C32" s="165"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="81"/>
+      <c r="F32" s="81"/>
+      <c r="G32" s="82"/>
       <c r="H32" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="I32" s="157"/>
-      <c r="J32" s="157"/>
-      <c r="K32" s="157"/>
+        <v>77</v>
+      </c>
+      <c r="I32" s="111"/>
+      <c r="J32" s="111"/>
+      <c r="K32" s="111"/>
       <c r="L32" s="43" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="M32" s="45"/>
       <c r="N32" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="O32" s="111"/>
+      <c r="P32" s="111"/>
+      <c r="Q32" s="111"/>
+      <c r="R32" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="S32" s="83"/>
+      <c r="T32" s="83"/>
+      <c r="U32" s="83"/>
+      <c r="V32" s="84"/>
+    </row>
+    <row r="33" spans="2:22" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="159" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="160"/>
+      <c r="D33" s="160"/>
+      <c r="E33" s="160"/>
+      <c r="F33" s="160"/>
+      <c r="G33" s="160"/>
+      <c r="H33" s="160"/>
+      <c r="I33" s="160"/>
+      <c r="J33" s="160"/>
+      <c r="K33" s="161"/>
+      <c r="L33" s="159" t="s">
+        <v>76</v>
+      </c>
+      <c r="M33" s="160"/>
+      <c r="N33" s="160"/>
+      <c r="O33" s="160"/>
+      <c r="P33" s="160"/>
+      <c r="Q33" s="160"/>
+      <c r="R33" s="160"/>
+      <c r="S33" s="160"/>
+      <c r="T33" s="160"/>
+      <c r="U33" s="160"/>
+      <c r="V33" s="161"/>
+    </row>
+    <row r="34" spans="2:22" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="162"/>
+      <c r="C34" s="163"/>
+      <c r="D34" s="163"/>
+      <c r="E34" s="163"/>
+      <c r="F34" s="163"/>
+      <c r="G34" s="163"/>
+      <c r="H34" s="163"/>
+      <c r="I34" s="163"/>
+      <c r="J34" s="163"/>
+      <c r="K34" s="164"/>
+      <c r="L34" s="162"/>
+      <c r="M34" s="163"/>
+      <c r="N34" s="163"/>
+      <c r="O34" s="163"/>
+      <c r="P34" s="163"/>
+      <c r="Q34" s="163"/>
+      <c r="R34" s="163"/>
+      <c r="S34" s="163"/>
+      <c r="T34" s="163"/>
+      <c r="U34" s="163"/>
+      <c r="V34" s="164"/>
+    </row>
+    <row r="35" spans="2:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="142" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="143"/>
+      <c r="D35" s="144"/>
+      <c r="E35" s="145"/>
+      <c r="F35" s="145"/>
+      <c r="G35" s="145"/>
+      <c r="H35" s="145"/>
+      <c r="I35" s="145"/>
+      <c r="J35" s="145"/>
+      <c r="K35" s="146"/>
+      <c r="L35" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="M35" s="145"/>
+      <c r="N35" s="145"/>
+      <c r="O35" s="145"/>
+      <c r="P35" s="145"/>
+      <c r="Q35" s="145"/>
+      <c r="R35" s="145"/>
+      <c r="S35" s="145"/>
+      <c r="T35" s="145"/>
+      <c r="U35" s="145"/>
+      <c r="V35" s="146"/>
+    </row>
+    <row r="36" spans="2:22" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="147" t="s">
         <v>65</v>
       </c>
-      <c r="O32" s="157"/>
-      <c r="P32" s="157"/>
-      <c r="Q32" s="157"/>
-      <c r="R32" s="43" t="s">
+      <c r="C36" s="148"/>
+      <c r="D36" s="149"/>
+      <c r="E36" s="129"/>
+      <c r="F36" s="129"/>
+      <c r="G36" s="129"/>
+      <c r="H36" s="129"/>
+      <c r="I36" s="129"/>
+      <c r="J36" s="129"/>
+      <c r="K36" s="150"/>
+      <c r="L36" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="S32" s="162"/>
-      <c r="T32" s="162"/>
-      <c r="U32" s="162"/>
-      <c r="V32" s="160"/>
-    </row>
-    <row r="33" spans="2:22" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="147" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="159"/>
-      <c r="D33" s="169"/>
-      <c r="E33" s="170"/>
-      <c r="F33" s="170"/>
-      <c r="G33" s="171"/>
-      <c r="H33" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="I33" s="80"/>
-      <c r="J33" s="80"/>
-      <c r="K33" s="80"/>
-      <c r="L33" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="M33" s="172"/>
-      <c r="N33" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="O33" s="80"/>
-      <c r="P33" s="80"/>
-      <c r="Q33" s="80"/>
-      <c r="R33" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="S33" s="173"/>
-      <c r="T33" s="173"/>
-      <c r="U33" s="173"/>
-      <c r="V33" s="174"/>
-    </row>
-    <row r="34" spans="2:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="163" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="164"/>
-      <c r="D34" s="164"/>
-      <c r="E34" s="164"/>
-      <c r="F34" s="164"/>
-      <c r="G34" s="164"/>
-      <c r="H34" s="164"/>
-      <c r="I34" s="164"/>
-      <c r="J34" s="164"/>
-      <c r="K34" s="165"/>
-      <c r="L34" s="163" t="s">
-        <v>76</v>
-      </c>
-      <c r="M34" s="164"/>
-      <c r="N34" s="164"/>
-      <c r="O34" s="164"/>
-      <c r="P34" s="164"/>
-      <c r="Q34" s="164"/>
-      <c r="R34" s="164"/>
-      <c r="S34" s="164"/>
-      <c r="T34" s="164"/>
-      <c r="U34" s="164"/>
-      <c r="V34" s="165"/>
-    </row>
-    <row r="35" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="166"/>
-      <c r="C35" s="167"/>
-      <c r="D35" s="167"/>
-      <c r="E35" s="167"/>
-      <c r="F35" s="167"/>
-      <c r="G35" s="167"/>
-      <c r="H35" s="167"/>
-      <c r="I35" s="167"/>
-      <c r="J35" s="167"/>
-      <c r="K35" s="168"/>
-      <c r="L35" s="166"/>
-      <c r="M35" s="167"/>
-      <c r="N35" s="167"/>
-      <c r="O35" s="167"/>
-      <c r="P35" s="167"/>
-      <c r="Q35" s="167"/>
-      <c r="R35" s="167"/>
-      <c r="S35" s="167"/>
-      <c r="T35" s="167"/>
-      <c r="U35" s="167"/>
-      <c r="V35" s="168"/>
-    </row>
-    <row r="36" spans="2:22" ht="31.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="142" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" s="143"/>
-      <c r="D36" s="144"/>
-      <c r="E36" s="145"/>
-      <c r="F36" s="145"/>
-      <c r="G36" s="145"/>
-      <c r="H36" s="145"/>
-      <c r="I36" s="145"/>
-      <c r="J36" s="145"/>
-      <c r="K36" s="146"/>
-      <c r="L36" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="M36" s="145"/>
-      <c r="N36" s="145"/>
-      <c r="O36" s="145"/>
-      <c r="P36" s="145"/>
-      <c r="Q36" s="145"/>
-      <c r="R36" s="145"/>
-      <c r="S36" s="145"/>
-      <c r="T36" s="145"/>
-      <c r="U36" s="145"/>
-      <c r="V36" s="146"/>
-    </row>
-    <row r="37" spans="2:22" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="147" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" s="148"/>
-      <c r="D37" s="149"/>
-      <c r="E37" s="124"/>
-      <c r="F37" s="124"/>
-      <c r="G37" s="124"/>
-      <c r="H37" s="124"/>
-      <c r="I37" s="124"/>
-      <c r="J37" s="124"/>
-      <c r="K37" s="150"/>
-      <c r="L37" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="M37" s="151"/>
-      <c r="N37" s="151"/>
-      <c r="O37" s="151"/>
-      <c r="P37" s="151"/>
-      <c r="Q37" s="151"/>
-      <c r="R37" s="151"/>
-      <c r="S37" s="151"/>
-      <c r="T37" s="151"/>
-      <c r="U37" s="151"/>
-      <c r="V37" s="125"/>
-    </row>
-    <row r="38" spans="2:22" ht="109.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="126" t="s">
+      <c r="M36" s="151"/>
+      <c r="N36" s="151"/>
+      <c r="O36" s="151"/>
+      <c r="P36" s="151"/>
+      <c r="Q36" s="151"/>
+      <c r="R36" s="151"/>
+      <c r="S36" s="151"/>
+      <c r="T36" s="151"/>
+      <c r="U36" s="151"/>
+      <c r="V36" s="130"/>
+    </row>
+    <row r="37" spans="2:22" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="169" t="s">
         <v>66</v>
       </c>
-      <c r="C38" s="127"/>
-      <c r="D38" s="127"/>
-      <c r="E38" s="127"/>
-      <c r="F38" s="127"/>
-      <c r="G38" s="127"/>
-      <c r="H38" s="127"/>
-      <c r="I38" s="127"/>
-      <c r="J38" s="127"/>
-      <c r="K38" s="127"/>
-      <c r="L38" s="127"/>
-      <c r="M38" s="127"/>
-      <c r="N38" s="127"/>
-      <c r="O38" s="127"/>
-      <c r="P38" s="127"/>
-      <c r="Q38" s="127"/>
-      <c r="R38" s="127"/>
-      <c r="S38" s="127"/>
-      <c r="T38" s="127"/>
-      <c r="U38" s="127"/>
-      <c r="V38" s="127"/>
-    </row>
+      <c r="C37" s="170"/>
+      <c r="D37" s="170"/>
+      <c r="E37" s="170"/>
+      <c r="F37" s="170"/>
+      <c r="G37" s="170"/>
+      <c r="H37" s="170"/>
+      <c r="I37" s="170"/>
+      <c r="J37" s="170"/>
+      <c r="K37" s="170"/>
+      <c r="L37" s="170"/>
+      <c r="M37" s="170"/>
+      <c r="N37" s="170"/>
+      <c r="O37" s="170"/>
+      <c r="P37" s="170"/>
+      <c r="Q37" s="170"/>
+      <c r="R37" s="170"/>
+      <c r="S37" s="170"/>
+      <c r="T37" s="170"/>
+      <c r="U37" s="170"/>
+      <c r="V37" s="171"/>
+    </row>
+    <row r="38" spans="2:22" ht="109.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="2:22" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="108">
+  <mergeCells count="103">
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:K35"/>
+    <mergeCell ref="M35:V35"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="D36:K36"/>
     <mergeCell ref="M36:V36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:K37"/>
-    <mergeCell ref="M37:V37"/>
     <mergeCell ref="B24:V24"/>
     <mergeCell ref="L30:M30"/>
     <mergeCell ref="N30:Q30"/>
@@ -4064,14 +4023,11 @@
     <mergeCell ref="I31:K31"/>
     <mergeCell ref="O31:Q31"/>
     <mergeCell ref="S31:V31"/>
+    <mergeCell ref="B33:K34"/>
+    <mergeCell ref="L33:V34"/>
     <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="O32:Q32"/>
     <mergeCell ref="I32:K32"/>
-    <mergeCell ref="O32:Q32"/>
-    <mergeCell ref="S32:V32"/>
-    <mergeCell ref="B34:K35"/>
-    <mergeCell ref="L34:V35"/>
-    <mergeCell ref="B33:C33"/>
     <mergeCell ref="N21:Q21"/>
     <mergeCell ref="R21:V21"/>
     <mergeCell ref="B29:V29"/>
@@ -4091,7 +4047,7 @@
     <mergeCell ref="M3:V3"/>
     <mergeCell ref="M4:V4"/>
     <mergeCell ref="B2:D3"/>
-    <mergeCell ref="B38:V38"/>
+    <mergeCell ref="B37:V37"/>
     <mergeCell ref="T9:V9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="N10:S10"/>
@@ -4109,12 +4065,6 @@
     <mergeCell ref="L7:N7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="E8:K8"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="R15:V15"/>
     <mergeCell ref="L8:N8"/>
     <mergeCell ref="C12:E13"/>
     <mergeCell ref="F12:F13"/>
@@ -4125,8 +4075,6 @@
     <mergeCell ref="N12:Q13"/>
     <mergeCell ref="R12:V13"/>
     <mergeCell ref="J13:K13"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
     <mergeCell ref="N17:Q17"/>
     <mergeCell ref="R17:V17"/>
     <mergeCell ref="C14:E14"/>
@@ -4134,10 +4082,14 @@
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="N14:Q14"/>
     <mergeCell ref="R14:V14"/>
-    <mergeCell ref="O33:Q33"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="S33:V33"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="R15:V15"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="S32:V32"/>
     <mergeCell ref="O7:V7"/>
     <mergeCell ref="O8:V8"/>
     <mergeCell ref="D31:G31"/>
@@ -4158,6 +4110,8 @@
     <mergeCell ref="N16:Q16"/>
     <mergeCell ref="R16:V16"/>
     <mergeCell ref="C17:E17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>